<commit_message>
New runs and general updates
</commit_message>
<xml_diff>
--- a/models/trv_scenario2.xlsx
+++ b/models/trv_scenario2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Beskrivning" sheetId="19" r:id="rId1"/>
@@ -1282,7 +1282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1707" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1708" uniqueCount="408">
   <si>
     <t>Drivmedelspris</t>
   </si>
@@ -2628,6 +2628,9 @@
   </si>
   <si>
     <t>Biofouel cost adjustment (before tax)</t>
+  </si>
+  <si>
+    <t>Förändring i utsläpp bilar</t>
   </si>
 </sst>
 </file>
@@ -5242,6 +5245,39 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5257,44 +5293,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5302,30 +5329,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5338,45 +5341,45 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5386,6 +5389,36 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5395,41 +5428,11 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="28">
@@ -5522,6 +5525,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5827,6 +5831,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6017,6 +6022,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6322,6 +6328,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -6512,6 +6519,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6817,6 +6825,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -7007,6 +7016,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7312,6 +7322,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10569,87 +10580,87 @@
     </row>
     <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:39" s="325" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="639" t="s">
+      <c r="A3" s="634" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="645" t="s">
+      <c r="B3" s="636" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="646"/>
-      <c r="D3" s="639" t="s">
+      <c r="C3" s="637"/>
+      <c r="D3" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="638"/>
-      <c r="F3" s="639" t="s">
+      <c r="E3" s="647"/>
+      <c r="F3" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="638"/>
-      <c r="H3" s="637" t="s">
+      <c r="G3" s="647"/>
+      <c r="H3" s="648" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="638"/>
-      <c r="K3" s="639" t="s">
+      <c r="I3" s="647"/>
+      <c r="K3" s="634" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="645" t="s">
+      <c r="L3" s="636" t="s">
         <v>240</v>
       </c>
-      <c r="M3" s="646"/>
-      <c r="N3" s="639" t="s">
+      <c r="M3" s="637"/>
+      <c r="N3" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="638"/>
-      <c r="P3" s="639" t="s">
+      <c r="O3" s="647"/>
+      <c r="P3" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="638"/>
-      <c r="R3" s="637" t="s">
+      <c r="Q3" s="647"/>
+      <c r="R3" s="648" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="638"/>
-      <c r="U3" s="639" t="s">
+      <c r="S3" s="647"/>
+      <c r="U3" s="634" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="645" t="s">
+      <c r="V3" s="636" t="s">
         <v>241</v>
       </c>
-      <c r="W3" s="646"/>
-      <c r="X3" s="639" t="s">
+      <c r="W3" s="637"/>
+      <c r="X3" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="638"/>
-      <c r="Z3" s="639" t="s">
+      <c r="Y3" s="647"/>
+      <c r="Z3" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="AA3" s="638"/>
-      <c r="AB3" s="637" t="s">
+      <c r="AA3" s="647"/>
+      <c r="AB3" s="648" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="638"/>
-      <c r="AE3" s="639" t="s">
+      <c r="AC3" s="647"/>
+      <c r="AE3" s="634" t="s">
         <v>67</v>
       </c>
-      <c r="AF3" s="645" t="s">
+      <c r="AF3" s="636" t="s">
         <v>238</v>
       </c>
-      <c r="AG3" s="646"/>
-      <c r="AH3" s="639" t="s">
+      <c r="AG3" s="637"/>
+      <c r="AH3" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="AI3" s="638"/>
-      <c r="AJ3" s="639" t="s">
+      <c r="AI3" s="647"/>
+      <c r="AJ3" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="AK3" s="638"/>
-      <c r="AL3" s="637" t="s">
+      <c r="AK3" s="647"/>
+      <c r="AL3" s="648" t="s">
         <v>66</v>
       </c>
-      <c r="AM3" s="638"/>
+      <c r="AM3" s="647"/>
     </row>
     <row r="4" spans="1:39" s="127" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="644"/>
-      <c r="B4" s="647"/>
-      <c r="C4" s="648"/>
+      <c r="A4" s="635"/>
+      <c r="B4" s="638"/>
+      <c r="C4" s="639"/>
       <c r="D4" s="265">
         <v>2030</v>
       </c>
@@ -10668,9 +10679,9 @@
       <c r="I4" s="266">
         <v>2040</v>
       </c>
-      <c r="K4" s="644"/>
-      <c r="L4" s="647"/>
-      <c r="M4" s="648"/>
+      <c r="K4" s="635"/>
+      <c r="L4" s="638"/>
+      <c r="M4" s="639"/>
       <c r="N4" s="265">
         <v>2030</v>
       </c>
@@ -10689,9 +10700,9 @@
       <c r="S4" s="266">
         <v>2040</v>
       </c>
-      <c r="U4" s="644"/>
-      <c r="V4" s="647"/>
-      <c r="W4" s="648"/>
+      <c r="U4" s="635"/>
+      <c r="V4" s="638"/>
+      <c r="W4" s="639"/>
       <c r="X4" s="265">
         <v>2030</v>
       </c>
@@ -10710,9 +10721,9 @@
       <c r="AC4" s="266">
         <v>2040</v>
       </c>
-      <c r="AE4" s="644"/>
-      <c r="AF4" s="647"/>
-      <c r="AG4" s="648"/>
+      <c r="AE4" s="635"/>
+      <c r="AF4" s="638"/>
+      <c r="AG4" s="639"/>
       <c r="AH4" s="265">
         <v>2030</v>
       </c>
@@ -10773,7 +10784,7 @@
       <c r="AM5" s="76"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="634" t="s">
+      <c r="A6" s="644" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="135" t="s">
@@ -10806,7 +10817,7 @@
         <f>Indata!I54</f>
         <v>19.161594511883557</v>
       </c>
-      <c r="K6" s="634" t="s">
+      <c r="K6" s="644" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="135" t="s">
@@ -10839,7 +10850,7 @@
         <f>'Modell - Drivmedelpriser'!J58</f>
         <v>19.161594511883557</v>
       </c>
-      <c r="U6" s="634" t="s">
+      <c r="U6" s="644" t="s">
         <v>0</v>
       </c>
       <c r="V6" s="135" t="s">
@@ -10872,7 +10883,7 @@
         <f t="shared" ref="AC6:AC7" si="4">S6</f>
         <v>19.161594511883557</v>
       </c>
-      <c r="AE6" s="634" t="s">
+      <c r="AE6" s="644" t="s">
         <v>0</v>
       </c>
       <c r="AF6" s="135" t="s">
@@ -10907,7 +10918,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="635"/>
+      <c r="A7" s="645"/>
       <c r="B7" s="136" t="s">
         <v>7</v>
       </c>
@@ -10938,7 +10949,7 @@
         <f>Indata!I55</f>
         <v>1.4034</v>
       </c>
-      <c r="K7" s="635"/>
+      <c r="K7" s="645"/>
       <c r="L7" s="136" t="s">
         <v>7</v>
       </c>
@@ -10969,7 +10980,7 @@
         <f>'Modell - Drivmedelpriser'!J84</f>
         <v>1.4034</v>
       </c>
-      <c r="U7" s="635"/>
+      <c r="U7" s="645"/>
       <c r="V7" s="136" t="s">
         <v>7</v>
       </c>
@@ -11000,7 +11011,7 @@
         <f t="shared" si="4"/>
         <v>1.4034</v>
       </c>
-      <c r="AE7" s="635"/>
+      <c r="AE7" s="645"/>
       <c r="AF7" s="136" t="s">
         <v>7</v>
       </c>
@@ -11033,7 +11044,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="636"/>
+      <c r="A8" s="646"/>
       <c r="B8" s="188" t="s">
         <v>244</v>
       </c>
@@ -11058,7 +11069,7 @@
       <c r="I8" s="287" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="636"/>
+      <c r="K8" s="646"/>
       <c r="L8" s="188" t="s">
         <v>244</v>
       </c>
@@ -11089,7 +11100,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="U8" s="636"/>
+      <c r="U8" s="646"/>
       <c r="V8" s="188" t="s">
         <v>244</v>
       </c>
@@ -11120,7 +11131,7 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AE8" s="636"/>
+      <c r="AE8" s="646"/>
       <c r="AF8" s="188" t="s">
         <v>244</v>
       </c>
@@ -13122,7 +13133,7 @@
       <c r="AM28" s="77"/>
     </row>
     <row r="29" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="634" t="s">
+      <c r="A29" s="644" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="135" t="s">
@@ -13155,7 +13166,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K29" s="634" t="s">
+      <c r="K29" s="644" t="s">
         <v>21</v>
       </c>
       <c r="L29" s="135" t="s">
@@ -13188,7 +13199,7 @@
         <f t="shared" ref="S29:S32" si="65">I29</f>
         <v>0</v>
       </c>
-      <c r="U29" s="634" t="s">
+      <c r="U29" s="644" t="s">
         <v>21</v>
       </c>
       <c r="V29" s="135" t="s">
@@ -13221,7 +13232,7 @@
         <f t="shared" ref="AC29:AC32" si="70">S29</f>
         <v>0</v>
       </c>
-      <c r="AE29" s="634" t="s">
+      <c r="AE29" s="644" t="s">
         <v>21</v>
       </c>
       <c r="AF29" s="135" t="s">
@@ -13256,7 +13267,7 @@
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A30" s="635"/>
+      <c r="A30" s="645"/>
       <c r="B30" s="136" t="s">
         <v>117</v>
       </c>
@@ -13287,7 +13298,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K30" s="635"/>
+      <c r="K30" s="645"/>
       <c r="L30" s="136" t="s">
         <v>117</v>
       </c>
@@ -13318,7 +13329,7 @@
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
-      <c r="U30" s="635"/>
+      <c r="U30" s="645"/>
       <c r="V30" s="136" t="s">
         <v>117</v>
       </c>
@@ -13349,7 +13360,7 @@
         <f t="shared" si="70"/>
         <v>0</v>
       </c>
-      <c r="AE30" s="635"/>
+      <c r="AE30" s="645"/>
       <c r="AF30" s="136" t="s">
         <v>117</v>
       </c>
@@ -13382,7 +13393,7 @@
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A31" s="635"/>
+      <c r="A31" s="645"/>
       <c r="B31" s="136" t="s">
         <v>118</v>
       </c>
@@ -13413,7 +13424,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K31" s="635"/>
+      <c r="K31" s="645"/>
       <c r="L31" s="136" t="s">
         <v>118</v>
       </c>
@@ -13444,7 +13455,7 @@
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
-      <c r="U31" s="635"/>
+      <c r="U31" s="645"/>
       <c r="V31" s="136" t="s">
         <v>118</v>
       </c>
@@ -13475,7 +13486,7 @@
         <f t="shared" si="70"/>
         <v>0</v>
       </c>
-      <c r="AE31" s="635"/>
+      <c r="AE31" s="645"/>
       <c r="AF31" s="136" t="s">
         <v>118</v>
       </c>
@@ -13508,7 +13519,7 @@
       </c>
     </row>
     <row r="32" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="636"/>
+      <c r="A32" s="646"/>
       <c r="B32" s="137" t="s">
         <v>119</v>
       </c>
@@ -13539,7 +13550,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K32" s="636"/>
+      <c r="K32" s="646"/>
       <c r="L32" s="137" t="s">
         <v>119</v>
       </c>
@@ -13570,7 +13581,7 @@
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
-      <c r="U32" s="636"/>
+      <c r="U32" s="646"/>
       <c r="V32" s="137" t="s">
         <v>119</v>
       </c>
@@ -13601,7 +13612,7 @@
         <f t="shared" si="70"/>
         <v>0</v>
       </c>
-      <c r="AE32" s="636"/>
+      <c r="AE32" s="646"/>
       <c r="AF32" s="137" t="s">
         <v>119</v>
       </c>
@@ -18482,6 +18493,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="AE6:AE8"/>
+    <mergeCell ref="AE11:AE20"/>
+    <mergeCell ref="U29:U32"/>
+    <mergeCell ref="AE29:AE32"/>
+    <mergeCell ref="U23:U26"/>
+    <mergeCell ref="AE23:AE26"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="AE88:AE91"/>
+    <mergeCell ref="AE74:AE76"/>
+    <mergeCell ref="AE77:AE79"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="K11:K20"/>
+    <mergeCell ref="AE71:AE73"/>
+    <mergeCell ref="AE83:AE85"/>
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="K36:K50"/>
+    <mergeCell ref="U36:U50"/>
+    <mergeCell ref="AE36:AE50"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="U11:U20"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="AF3:AG4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AE92:AE96"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C4"/>
@@ -18498,40 +18543,6 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="K23:K26"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="AF3:AG4"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AE88:AE91"/>
-    <mergeCell ref="AE74:AE76"/>
-    <mergeCell ref="AE77:AE79"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="K11:K20"/>
-    <mergeCell ref="AE71:AE73"/>
-    <mergeCell ref="AE83:AE85"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="K36:K50"/>
-    <mergeCell ref="U36:U50"/>
-    <mergeCell ref="AE36:AE50"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="U11:U20"/>
-    <mergeCell ref="AE6:AE8"/>
-    <mergeCell ref="AE11:AE20"/>
-    <mergeCell ref="U29:U32"/>
-    <mergeCell ref="AE29:AE32"/>
-    <mergeCell ref="U23:U26"/>
-    <mergeCell ref="AE23:AE26"/>
-    <mergeCell ref="U6:U8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18545,11 +18556,11 @@
   </sheetPr>
   <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="7" topLeftCell="D56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="F38" sqref="F38"/>
+      <selection pane="bottomRight" activeCell="J73" sqref="J73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18599,18 +18610,18 @@
       <c r="A5" s="131"/>
       <c r="B5" s="132"/>
       <c r="C5" s="132"/>
-      <c r="D5" s="598" t="s">
+      <c r="D5" s="586" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="599"/>
-      <c r="F5" s="598" t="s">
+      <c r="E5" s="587"/>
+      <c r="F5" s="586" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="599"/>
-      <c r="H5" s="598" t="s">
+      <c r="G5" s="587"/>
+      <c r="H5" s="586" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="599"/>
+      <c r="I5" s="587"/>
       <c r="J5" s="594" t="s">
         <v>15</v>
       </c>
@@ -18630,18 +18641,18 @@
       </c>
       <c r="B6" s="138"/>
       <c r="C6" s="139"/>
-      <c r="D6" s="600" t="s">
+      <c r="D6" s="590" t="s">
         <v>337</v>
       </c>
-      <c r="E6" s="601"/>
-      <c r="F6" s="602" t="s">
+      <c r="E6" s="591"/>
+      <c r="F6" s="592" t="s">
         <v>382</v>
       </c>
-      <c r="G6" s="603"/>
-      <c r="H6" s="602" t="s">
+      <c r="G6" s="593"/>
+      <c r="H6" s="592" t="s">
         <v>382</v>
       </c>
-      <c r="I6" s="603"/>
+      <c r="I6" s="593"/>
       <c r="J6" s="65"/>
       <c r="K6" s="66"/>
       <c r="L6" s="66"/>
@@ -18736,7 +18747,7 @@
       <c r="S8" s="127"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="591" t="s">
+      <c r="A9" s="588" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="106" t="s">
@@ -18768,7 +18779,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="592"/>
+      <c r="A10" s="589"/>
       <c r="B10" s="43" t="s">
         <v>12</v>
       </c>
@@ -18798,7 +18809,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="592"/>
+      <c r="A11" s="589"/>
       <c r="B11" s="43" t="s">
         <v>13</v>
       </c>
@@ -18828,7 +18839,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="592"/>
+      <c r="A12" s="589"/>
       <c r="B12" s="43" t="s">
         <v>37</v>
       </c>
@@ -18858,7 +18869,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="591" t="s">
+      <c r="A13" s="588" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="106" t="s">
@@ -18890,7 +18901,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="593"/>
+      <c r="A14" s="596"/>
       <c r="B14" s="107" t="s">
         <v>9</v>
       </c>
@@ -18920,7 +18931,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="591" t="s">
+      <c r="A15" s="588" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="106" t="s">
@@ -18952,7 +18963,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="593"/>
+      <c r="A16" s="596"/>
       <c r="B16" s="107" t="s">
         <v>324</v>
       </c>
@@ -19055,7 +19066,7 @@
       <c r="S18" s="127"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="591" t="s">
+      <c r="A19" s="588" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="106" t="s">
@@ -19087,7 +19098,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="593"/>
+      <c r="A20" s="596"/>
       <c r="B20" s="107" t="s">
         <v>324</v>
       </c>
@@ -19117,7 +19128,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="592" t="s">
+      <c r="A21" s="589" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="106" t="s">
@@ -19149,7 +19160,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="593"/>
+      <c r="A22" s="596"/>
       <c r="B22" s="107" t="s">
         <v>324</v>
       </c>
@@ -19252,7 +19263,7 @@
       <c r="S24" s="127"/>
     </row>
     <row r="25" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="591" t="s">
+      <c r="A25" s="588" t="s">
         <v>150</v>
       </c>
       <c r="B25" s="106" t="s">
@@ -19299,7 +19310,7 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="592"/>
+      <c r="A26" s="589"/>
       <c r="B26" s="43" t="s">
         <v>9</v>
       </c>
@@ -19344,7 +19355,7 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="593"/>
+      <c r="A27" s="596"/>
       <c r="B27" s="107" t="s">
         <v>7</v>
       </c>
@@ -19436,7 +19447,7 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="591" t="s">
+      <c r="A29" s="588" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="106" t="s">
@@ -19483,7 +19494,7 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="592"/>
+      <c r="A30" s="589"/>
       <c r="B30" s="43" t="s">
         <v>9</v>
       </c>
@@ -19528,7 +19539,7 @@
       <c r="S30" s="26"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="593"/>
+      <c r="A31" s="596"/>
       <c r="B31" s="107" t="s">
         <v>7</v>
       </c>
@@ -19573,7 +19584,7 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="586" t="s">
+      <c r="A32" s="597" t="s">
         <v>0</v>
       </c>
       <c r="B32" s="106" t="s">
@@ -19611,7 +19622,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="596"/>
+      <c r="A33" s="602"/>
       <c r="B33" s="43" t="s">
         <v>9</v>
       </c>
@@ -19647,7 +19658,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="596"/>
+      <c r="A34" s="602"/>
       <c r="B34" s="43" t="s">
         <v>7</v>
       </c>
@@ -19683,7 +19694,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="587"/>
+      <c r="A35" s="598"/>
       <c r="B35" s="107" t="s">
         <v>20</v>
       </c>
@@ -19846,7 +19857,7 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="588" t="s">
+      <c r="A39" s="599" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="106" t="s">
@@ -19892,7 +19903,7 @@
       <c r="S39" s="26"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="597"/>
+      <c r="A40" s="603"/>
       <c r="B40" s="107" t="s">
         <v>29</v>
       </c>
@@ -19978,7 +19989,7 @@
       <c r="S41" s="127"/>
     </row>
     <row r="42" spans="1:19" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="586" t="s">
+      <c r="A42" s="597" t="s">
         <v>150</v>
       </c>
       <c r="B42" s="106" t="s">
@@ -20025,7 +20036,7 @@
       <c r="S42" s="26"/>
     </row>
     <row r="43" spans="1:19" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="596"/>
+      <c r="A43" s="602"/>
       <c r="B43" s="43" t="s">
         <v>117</v>
       </c>
@@ -20070,7 +20081,7 @@
       <c r="S43" s="26"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="589"/>
+      <c r="A44" s="600"/>
       <c r="B44" s="43" t="s">
         <v>118</v>
       </c>
@@ -20115,7 +20126,7 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="589"/>
+      <c r="A45" s="600"/>
       <c r="B45" s="43" t="s">
         <v>119</v>
       </c>
@@ -20160,7 +20171,7 @@
       <c r="S45" s="26"/>
     </row>
     <row r="46" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="586" t="s">
+      <c r="A46" s="597" t="s">
         <v>381</v>
       </c>
       <c r="B46" s="106" t="s">
@@ -20207,7 +20218,7 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="596"/>
+      <c r="A47" s="602"/>
       <c r="B47" s="43" t="s">
         <v>117</v>
       </c>
@@ -20252,7 +20263,7 @@
       <c r="S47" s="26"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="589"/>
+      <c r="A48" s="600"/>
       <c r="B48" s="43" t="s">
         <v>118</v>
       </c>
@@ -20297,7 +20308,7 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="589"/>
+      <c r="A49" s="600"/>
       <c r="B49" s="43" t="s">
         <v>119</v>
       </c>
@@ -20342,7 +20353,7 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="586" t="s">
+      <c r="A50" s="597" t="s">
         <v>380</v>
       </c>
       <c r="B50" s="106" t="s">
@@ -20389,7 +20400,7 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="596"/>
+      <c r="A51" s="602"/>
       <c r="B51" s="43" t="s">
         <v>117</v>
       </c>
@@ -20434,7 +20445,7 @@
       <c r="S51" s="26"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" s="589"/>
+      <c r="A52" s="600"/>
       <c r="B52" s="43" t="s">
         <v>118</v>
       </c>
@@ -20479,7 +20490,7 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="590"/>
+      <c r="A53" s="601"/>
       <c r="B53" s="107" t="s">
         <v>119</v>
       </c>
@@ -20524,7 +20535,7 @@
       <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="596" t="s">
+      <c r="A54" s="602" t="s">
         <v>0</v>
       </c>
       <c r="B54" s="43" t="s">
@@ -20562,7 +20573,7 @@
       </c>
     </row>
     <row r="55" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="596"/>
+      <c r="A55" s="602"/>
       <c r="B55" s="43" t="s">
         <v>7</v>
       </c>
@@ -20598,7 +20609,7 @@
       </c>
     </row>
     <row r="56" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="588" t="s">
+      <c r="A56" s="599" t="s">
         <v>17</v>
       </c>
       <c r="B56" s="342" t="s">
@@ -20636,7 +20647,7 @@
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="589"/>
+      <c r="A57" s="600"/>
       <c r="B57" s="43" t="s">
         <v>116</v>
       </c>
@@ -20681,7 +20692,7 @@
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="589"/>
+      <c r="A58" s="600"/>
       <c r="B58" s="43" t="s">
         <v>117</v>
       </c>
@@ -20726,7 +20737,7 @@
       <c r="S58" s="26"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="589"/>
+      <c r="A59" s="600"/>
       <c r="B59" s="43" t="s">
         <v>118</v>
       </c>
@@ -20771,7 +20782,7 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="590"/>
+      <c r="A60" s="601"/>
       <c r="B60" s="107" t="s">
         <v>119</v>
       </c>
@@ -20891,7 +20902,7 @@
       <c r="K62" s="595"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="586" t="s">
+      <c r="A63" s="597" t="s">
         <v>312</v>
       </c>
       <c r="B63" s="106" t="s">
@@ -20929,7 +20940,7 @@
       </c>
     </row>
     <row r="64" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="587"/>
+      <c r="A64" s="598"/>
       <c r="B64" s="107" t="s">
         <v>7</v>
       </c>
@@ -21048,6 +21059,15 @@
         <v>4.0914621637292967</v>
       </c>
     </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C74" s="40" t="s">
+        <v>407</v>
+      </c>
+      <c r="D74" s="40">
+        <f>Resultat!F37/'Indata - Utsläpp'!B15-1</f>
+        <v>-0.73481851843620594</v>
+      </c>
+    </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B78" s="40" t="s">
         <v>395</v>
@@ -21072,24 +21092,6 @@
     <protectedRange algorithmName="SHA-512" hashValue="bhbLMjBtLJkCl6+oRAIq98NZkcBAWzm8GjbRfoftLGnxxPl6tbwDiFe+9aTX2EHNMDT88cd1rnVmqQcow+/x8w==" saltValue="u4cWX+yqQiFBZXUHKrq6Og==" spinCount="100000" sqref="F9:I23" name="Indata"/>
   </protectedRanges>
   <mergeCells count="28">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A63:A64"/>
     <mergeCell ref="A56:A60"/>
     <mergeCell ref="A29:A31"/>
@@ -21100,6 +21102,24 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -21133,10 +21153,10 @@
   <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21222,18 +21242,18 @@
       <c r="C4" s="132" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="598" t="s">
+      <c r="D4" s="586" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="599"/>
-      <c r="F4" s="598" t="s">
+      <c r="E4" s="587"/>
+      <c r="F4" s="586" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="599"/>
-      <c r="H4" s="598" t="s">
+      <c r="G4" s="587"/>
+      <c r="H4" s="586" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="599"/>
+      <c r="I4" s="587"/>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
       <c r="L4" s="40"/>
@@ -21249,21 +21269,21 @@
       </c>
       <c r="B5" s="290"/>
       <c r="C5" s="291"/>
-      <c r="D5" s="604" t="str">
+      <c r="D5" s="612" t="str">
         <f>Indata!D6</f>
         <v>Beslutad politik</v>
       </c>
-      <c r="E5" s="605"/>
-      <c r="F5" s="604" t="str">
+      <c r="E5" s="613"/>
+      <c r="F5" s="612" t="str">
         <f>Indata!F6</f>
         <v>Här kan användaren beskriva sitt scenario, t.ex. "Biodrivmedelsscenario"</v>
       </c>
-      <c r="G5" s="605"/>
-      <c r="H5" s="604" t="str">
+      <c r="G5" s="613"/>
+      <c r="H5" s="612" t="str">
         <f>Indata!H6</f>
         <v>Här kan användaren beskriva sitt scenario, t.ex. "Biodrivmedelsscenario"</v>
       </c>
-      <c r="I5" s="605"/>
+      <c r="I5" s="613"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
       <c r="L5" s="66"/>
@@ -21311,7 +21331,7 @@
       <c r="Q6" s="127"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="606" t="s">
+      <c r="A7" s="607" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="292" t="s">
@@ -21445,7 +21465,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="607"/>
+      <c r="A11" s="609"/>
       <c r="B11" s="294" t="s">
         <v>185</v>
       </c>
@@ -21478,7 +21498,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="606" t="s">
+      <c r="A12" s="607" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="292" t="s">
@@ -21613,7 +21633,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="607"/>
+      <c r="A16" s="609"/>
       <c r="B16" s="294" t="s">
         <v>323</v>
       </c>
@@ -21646,7 +21666,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="606" t="s">
+      <c r="A17" s="607" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="292" t="s">
@@ -21681,7 +21701,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="607"/>
+      <c r="A18" s="609"/>
       <c r="B18" s="294" t="s">
         <v>324</v>
       </c>
@@ -21749,7 +21769,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="606" t="s">
+      <c r="A20" s="607" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="292" t="s">
@@ -21954,7 +21974,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="607"/>
+      <c r="A26" s="609"/>
       <c r="B26" s="392" t="s">
         <v>359</v>
       </c>
@@ -21987,7 +22007,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="606" t="s">
+      <c r="A27" s="607" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="292" t="s">
@@ -22226,7 +22246,7 @@
       <c r="J33" s="381"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="607"/>
+      <c r="A34" s="609"/>
       <c r="B34" s="392" t="s">
         <v>338</v>
       </c>
@@ -22295,7 +22315,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="607"/>
+      <c r="A36" s="609"/>
       <c r="B36" s="294" t="s">
         <v>324</v>
       </c>
@@ -22328,7 +22348,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="612" t="s">
+      <c r="A37" s="610" t="s">
         <v>279</v>
       </c>
       <c r="B37" s="292" t="s">
@@ -22363,7 +22383,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="613"/>
+      <c r="A38" s="611"/>
       <c r="B38" s="293" t="s">
         <v>324</v>
       </c>
@@ -22396,7 +22416,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="613"/>
+      <c r="A39" s="611"/>
       <c r="B39" s="293" t="s">
         <v>315</v>
       </c>
@@ -22423,7 +22443,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="613"/>
+      <c r="A40" s="611"/>
       <c r="B40" s="391" t="s">
         <v>16</v>
       </c>
@@ -22456,7 +22476,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="613"/>
+      <c r="A41" s="611"/>
       <c r="B41" s="518" t="s">
         <v>362</v>
       </c>
@@ -22489,7 +22509,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="606" t="s">
+      <c r="A42" s="607" t="s">
         <v>276</v>
       </c>
       <c r="B42" s="292" t="s">
@@ -22760,7 +22780,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="606" t="s">
+      <c r="A50" s="607" t="s">
         <v>271</v>
       </c>
       <c r="B50" s="292" t="s">
@@ -22894,7 +22914,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="609" t="s">
+      <c r="A54" s="604" t="s">
         <v>130</v>
       </c>
       <c r="B54" s="292" t="s">
@@ -22930,7 +22950,7 @@
       <c r="J54" s="381"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="610"/>
+      <c r="A55" s="605"/>
       <c r="B55" s="293" t="s">
         <v>320</v>
       </c>
@@ -22965,7 +22985,7 @@
       <c r="K55" s="381"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="610"/>
+      <c r="A56" s="605"/>
       <c r="B56" s="293" t="s">
         <v>104</v>
       </c>
@@ -23000,7 +23020,7 @@
       <c r="K56" s="381"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="610"/>
+      <c r="A57" s="605"/>
       <c r="B57" s="293" t="s">
         <v>317</v>
       </c>
@@ -23039,7 +23059,7 @@
       <c r="O57" s="521"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="610"/>
+      <c r="A58" s="605"/>
       <c r="B58" s="293" t="s">
         <v>318</v>
       </c>
@@ -23074,7 +23094,7 @@
       <c r="K58" s="381"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="610"/>
+      <c r="A59" s="605"/>
       <c r="B59" s="293" t="s">
         <v>319</v>
       </c>
@@ -23110,7 +23130,7 @@
       <c r="O59" s="381"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="610"/>
+      <c r="A60" s="605"/>
       <c r="B60" s="391" t="s">
         <v>198</v>
       </c>
@@ -23149,7 +23169,7 @@
       <c r="O60" s="521"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="610"/>
+      <c r="A61" s="605"/>
       <c r="B61" s="391" t="s">
         <v>199</v>
       </c>
@@ -23184,7 +23204,7 @@
       <c r="K61" s="381"/>
     </row>
     <row r="62" spans="1:15" s="381" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="610"/>
+      <c r="A62" s="605"/>
       <c r="B62" s="391" t="s">
         <v>200</v>
       </c>
@@ -23217,7 +23237,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="611"/>
+      <c r="A63" s="606"/>
       <c r="B63" s="392" t="s">
         <v>364</v>
       </c>
@@ -23252,7 +23272,7 @@
       <c r="K63" s="381"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="610" t="s">
+      <c r="A64" s="605" t="s">
         <v>245</v>
       </c>
       <c r="B64" s="293" t="s">
@@ -23287,7 +23307,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="610"/>
+      <c r="A65" s="605"/>
       <c r="B65" s="293" t="s">
         <v>197</v>
       </c>
@@ -23320,7 +23340,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="610"/>
+      <c r="A66" s="605"/>
       <c r="B66" s="293" t="s">
         <v>104</v>
       </c>
@@ -23353,7 +23373,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="610"/>
+      <c r="A67" s="605"/>
       <c r="B67" s="293" t="s">
         <v>322</v>
       </c>
@@ -23386,7 +23406,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="610"/>
+      <c r="A68" s="605"/>
       <c r="B68" s="293" t="s">
         <v>321</v>
       </c>
@@ -23419,7 +23439,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="610"/>
+      <c r="A69" s="605"/>
       <c r="B69" s="293" t="s">
         <v>323</v>
       </c>
@@ -23452,7 +23472,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="610"/>
+      <c r="A70" s="605"/>
       <c r="B70" s="391" t="s">
         <v>198</v>
       </c>
@@ -23485,7 +23505,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="610"/>
+      <c r="A71" s="605"/>
       <c r="B71" s="391" t="s">
         <v>199</v>
       </c>
@@ -23518,7 +23538,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="611"/>
+      <c r="A72" s="606"/>
       <c r="B72" s="392" t="s">
         <v>200</v>
       </c>
@@ -23551,7 +23571,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="609" t="s">
+      <c r="A73" s="604" t="s">
         <v>203</v>
       </c>
       <c r="B73" s="292" t="s">
@@ -23586,7 +23606,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="610"/>
+      <c r="A74" s="605"/>
       <c r="B74" s="293" t="s">
         <v>324</v>
       </c>
@@ -23619,7 +23639,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="611"/>
+      <c r="A75" s="606"/>
       <c r="B75" s="392" t="s">
         <v>278</v>
       </c>
@@ -23652,7 +23672,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="609" t="s">
+      <c r="A76" s="604" t="s">
         <v>204</v>
       </c>
       <c r="B76" s="292" t="s">
@@ -23687,7 +23707,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="610"/>
+      <c r="A77" s="605"/>
       <c r="B77" s="293" t="s">
         <v>324</v>
       </c>
@@ -23720,7 +23740,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="611"/>
+      <c r="A78" s="606"/>
       <c r="B78" s="392" t="s">
         <v>278</v>
       </c>
@@ -23761,6 +23781,17 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
     <mergeCell ref="A73:A75"/>
     <mergeCell ref="A76:A78"/>
     <mergeCell ref="A27:A34"/>
@@ -23770,17 +23801,6 @@
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23829,7 +23849,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24664,7 +24684,7 @@
   <dimension ref="A1:T42"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25947,13 +25967,13 @@
       <c r="O3" s="127"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="588" t="s">
+      <c r="A4" s="599" t="s">
         <v>294</v>
       </c>
-      <c r="B4" s="621" t="s">
+      <c r="B4" s="620" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="622"/>
+      <c r="C4" s="621"/>
       <c r="D4" s="326">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -25974,11 +25994,11 @@
       <c r="O4" s="40"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="618"/>
-      <c r="B5" s="623" t="s">
+      <c r="A5" s="624"/>
+      <c r="B5" s="622" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="624"/>
+      <c r="C5" s="623"/>
       <c r="D5" s="326">
         <v>-0.05</v>
       </c>
@@ -25999,11 +26019,11 @@
       <c r="O5" s="40"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="618"/>
-      <c r="B6" s="623" t="s">
+      <c r="A6" s="624"/>
+      <c r="B6" s="622" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="624"/>
+      <c r="C6" s="623"/>
       <c r="D6" s="326">
         <v>0</v>
       </c>
@@ -26024,11 +26044,11 @@
       <c r="O6" s="40"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="618"/>
-      <c r="B7" s="623" t="s">
+      <c r="A7" s="624"/>
+      <c r="B7" s="622" t="s">
         <v>177</v>
       </c>
-      <c r="C7" s="624"/>
+      <c r="C7" s="623"/>
       <c r="D7" s="326">
         <v>-0.1</v>
       </c>
@@ -26049,11 +26069,11 @@
       <c r="O7" s="40"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="618"/>
-      <c r="B8" s="623" t="s">
+      <c r="A8" s="624"/>
+      <c r="B8" s="622" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="624"/>
+      <c r="C8" s="623"/>
       <c r="D8" s="326">
         <v>-0.2</v>
       </c>
@@ -26074,11 +26094,11 @@
       <c r="O8" s="40"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="597"/>
-      <c r="B9" s="619" t="s">
+      <c r="A9" s="603"/>
+      <c r="B9" s="618" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="620"/>
+      <c r="C9" s="619"/>
       <c r="D9" s="328">
         <f>Indata!D78</f>
         <v>-0.22</v>
@@ -26100,7 +26120,7 @@
       <c r="O9" s="40"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="591" t="s">
+      <c r="A10" s="588" t="s">
         <v>265</v>
       </c>
       <c r="B10" s="106" t="s">
@@ -26129,7 +26149,7 @@
       <c r="O10" s="40"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="592"/>
+      <c r="A11" s="589"/>
       <c r="B11" s="43" t="s">
         <v>9</v>
       </c>
@@ -26156,7 +26176,7 @@
       <c r="O11" s="40"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="592" t="s">
+      <c r="A12" s="589" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="43" t="s">
@@ -26185,7 +26205,7 @@
       <c r="O12" s="40"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="591" t="s">
+      <c r="A13" s="588" t="s">
         <v>266</v>
       </c>
       <c r="B13" s="106" t="s">
@@ -26214,7 +26234,7 @@
       <c r="O13" s="40"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="592"/>
+      <c r="A14" s="589"/>
       <c r="B14" s="43" t="s">
         <v>286</v>
       </c>
@@ -26241,7 +26261,7 @@
       <c r="O14" s="40"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="592" t="s">
+      <c r="A15" s="589" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="43" t="s">
@@ -26270,7 +26290,7 @@
       <c r="O15" s="40"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="591" t="s">
+      <c r="A16" s="588" t="s">
         <v>272</v>
       </c>
       <c r="B16" s="106" t="s">
@@ -26299,7 +26319,7 @@
       <c r="O16" s="40"/>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="592"/>
+      <c r="A17" s="589"/>
       <c r="B17" s="43" t="s">
         <v>286</v>
       </c>
@@ -26326,7 +26346,7 @@
       <c r="O17" s="40"/>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="593" t="s">
+      <c r="A18" s="596" t="s">
         <v>68</v>
       </c>
       <c r="B18" s="107" t="s">
@@ -26355,7 +26375,7 @@
       <c r="O18" s="40"/>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="610" t="s">
+      <c r="A19" s="605" t="s">
         <v>273</v>
       </c>
       <c r="B19" s="293" t="s">
@@ -26384,7 +26404,7 @@
       <c r="O19" s="40"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="610"/>
+      <c r="A20" s="605"/>
       <c r="B20" s="293" t="s">
         <v>296</v>
       </c>
@@ -26411,7 +26431,7 @@
       <c r="O20" s="40"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="586" t="s">
+      <c r="A21" s="597" t="s">
         <v>95</v>
       </c>
       <c r="B21" s="106" t="s">
@@ -26440,7 +26460,7 @@
       <c r="O21" s="40"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="596"/>
+      <c r="A22" s="602"/>
       <c r="B22" s="43" t="s">
         <v>97</v>
       </c>
@@ -26467,7 +26487,7 @@
       <c r="O22" s="40"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="596"/>
+      <c r="A23" s="602"/>
       <c r="B23" s="43" t="s">
         <v>134</v>
       </c>
@@ -26494,7 +26514,7 @@
       <c r="O23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="596"/>
+      <c r="A24" s="602"/>
       <c r="B24" s="43" t="s">
         <v>98</v>
       </c>
@@ -26521,7 +26541,7 @@
       <c r="O24" s="40"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="596"/>
+      <c r="A25" s="602"/>
       <c r="B25" s="43" t="s">
         <v>135</v>
       </c>
@@ -26548,7 +26568,7 @@
       <c r="O25" s="40"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="587"/>
+      <c r="A26" s="598"/>
       <c r="B26" s="107" t="s">
         <v>100</v>
       </c>
@@ -26576,6 +26596,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A4:A9"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B4:C4"/>
@@ -26583,11 +26608,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A4:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26601,7 +26621,7 @@
   </sheetPr>
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -26631,25 +26651,25 @@
       <c r="N1" s="40"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="628" t="s">
+      <c r="A2" s="625" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="628"/>
-      <c r="C2" s="628"/>
-      <c r="D2" s="628"/>
-      <c r="E2" s="628"/>
-      <c r="F2" s="628"/>
-      <c r="G2" s="628"/>
-      <c r="H2" s="628"/>
-      <c r="I2" s="628"/>
-      <c r="J2" s="628"/>
+      <c r="B2" s="625"/>
+      <c r="C2" s="625"/>
+      <c r="D2" s="625"/>
+      <c r="E2" s="625"/>
+      <c r="F2" s="625"/>
+      <c r="G2" s="625"/>
+      <c r="H2" s="625"/>
+      <c r="I2" s="625"/>
+      <c r="J2" s="625"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="629" t="s">
+      <c r="A3" s="626" t="s">
         <v>355</v>
       </c>
-      <c r="B3" s="630"/>
-      <c r="C3" s="630"/>
+      <c r="B3" s="627"/>
+      <c r="C3" s="627"/>
       <c r="D3" s="197"/>
       <c r="E3" s="197"/>
       <c r="F3" s="197"/>
@@ -26726,18 +26746,18 @@
       <c r="B7" s="194"/>
       <c r="C7" s="194"/>
       <c r="D7" s="194"/>
-      <c r="E7" s="625" t="s">
+      <c r="E7" s="630" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="626"/>
-      <c r="G7" s="625" t="s">
+      <c r="F7" s="629"/>
+      <c r="G7" s="630" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="626"/>
-      <c r="I7" s="627" t="s">
+      <c r="H7" s="629"/>
+      <c r="I7" s="628" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="626"/>
+      <c r="J7" s="629"/>
       <c r="L7" s="26" t="s">
         <v>403</v>
       </c>
@@ -27353,18 +27373,18 @@
       <c r="B26" s="194"/>
       <c r="C26" s="194"/>
       <c r="D26" s="194"/>
-      <c r="E26" s="625" t="s">
+      <c r="E26" s="630" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="626"/>
-      <c r="G26" s="625" t="s">
+      <c r="F26" s="629"/>
+      <c r="G26" s="630" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="626"/>
-      <c r="I26" s="627" t="s">
+      <c r="H26" s="629"/>
+      <c r="I26" s="628" t="s">
         <v>66</v>
       </c>
-      <c r="J26" s="626"/>
+      <c r="J26" s="629"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="196" t="s">
@@ -27963,18 +27983,18 @@
       <c r="B45" s="194"/>
       <c r="C45" s="194"/>
       <c r="D45" s="194"/>
-      <c r="E45" s="625" t="s">
+      <c r="E45" s="630" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="626"/>
-      <c r="G45" s="625" t="s">
+      <c r="F45" s="629"/>
+      <c r="G45" s="630" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="626"/>
-      <c r="I45" s="627" t="s">
+      <c r="H45" s="629"/>
+      <c r="I45" s="628" t="s">
         <v>66</v>
       </c>
-      <c r="J45" s="626"/>
+      <c r="J45" s="629"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="196" t="s">
@@ -28565,18 +28585,18 @@
       <c r="B64" s="194"/>
       <c r="C64" s="194"/>
       <c r="D64" s="194"/>
-      <c r="E64" s="625" t="s">
+      <c r="E64" s="630" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="626"/>
-      <c r="G64" s="625" t="s">
+      <c r="F64" s="629"/>
+      <c r="G64" s="630" t="s">
         <v>65</v>
       </c>
-      <c r="H64" s="626"/>
-      <c r="I64" s="627" t="s">
+      <c r="H64" s="629"/>
+      <c r="I64" s="628" t="s">
         <v>66</v>
       </c>
-      <c r="J64" s="626"/>
+      <c r="J64" s="629"/>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="196" t="s">
@@ -28966,18 +28986,18 @@
       <c r="B77" s="194"/>
       <c r="C77" s="194"/>
       <c r="D77" s="194"/>
-      <c r="E77" s="625" t="s">
+      <c r="E77" s="630" t="s">
         <v>64</v>
       </c>
-      <c r="F77" s="626"/>
-      <c r="G77" s="625" t="s">
+      <c r="F77" s="629"/>
+      <c r="G77" s="630" t="s">
         <v>65</v>
       </c>
-      <c r="H77" s="626"/>
-      <c r="I77" s="627" t="s">
+      <c r="H77" s="629"/>
+      <c r="I77" s="628" t="s">
         <v>66</v>
       </c>
-      <c r="J77" s="626"/>
+      <c r="J77" s="629"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="196" t="s">
@@ -29362,11 +29382,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
     <mergeCell ref="G77:H77"/>
     <mergeCell ref="I77:J77"/>
     <mergeCell ref="E7:F7"/>
@@ -29379,6 +29394,11 @@
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29393,9 +29413,9 @@
   </sheetPr>
   <dimension ref="A1:AM92"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="O1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ55" sqref="AJ55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29429,87 +29449,87 @@
     </row>
     <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:39" s="325" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="639" t="s">
+      <c r="A3" s="634" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="645" t="s">
+      <c r="B3" s="636" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="646"/>
-      <c r="D3" s="639" t="s">
+      <c r="C3" s="637"/>
+      <c r="D3" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="638"/>
-      <c r="F3" s="639" t="s">
+      <c r="E3" s="647"/>
+      <c r="F3" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="638"/>
-      <c r="H3" s="637" t="s">
+      <c r="G3" s="647"/>
+      <c r="H3" s="648" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="638"/>
-      <c r="K3" s="639" t="s">
+      <c r="I3" s="647"/>
+      <c r="K3" s="634" t="s">
         <v>67</v>
       </c>
       <c r="L3" s="640" t="s">
         <v>237</v>
       </c>
       <c r="M3" s="641"/>
-      <c r="N3" s="639" t="s">
+      <c r="N3" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="638"/>
-      <c r="P3" s="639" t="s">
+      <c r="O3" s="647"/>
+      <c r="P3" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="638"/>
-      <c r="R3" s="637" t="s">
+      <c r="Q3" s="647"/>
+      <c r="R3" s="648" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="638"/>
-      <c r="U3" s="639" t="s">
+      <c r="S3" s="647"/>
+      <c r="U3" s="634" t="s">
         <v>67</v>
       </c>
       <c r="V3" s="640" t="s">
         <v>227</v>
       </c>
       <c r="W3" s="641"/>
-      <c r="X3" s="639" t="s">
+      <c r="X3" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="638"/>
-      <c r="Z3" s="639" t="s">
+      <c r="Y3" s="647"/>
+      <c r="Z3" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="AA3" s="638"/>
-      <c r="AB3" s="637" t="s">
+      <c r="AA3" s="647"/>
+      <c r="AB3" s="648" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="638"/>
-      <c r="AE3" s="639" t="s">
+      <c r="AC3" s="647"/>
+      <c r="AE3" s="634" t="s">
         <v>67</v>
       </c>
       <c r="AF3" s="640" t="s">
         <v>238</v>
       </c>
       <c r="AG3" s="641"/>
-      <c r="AH3" s="639" t="s">
+      <c r="AH3" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="AI3" s="638"/>
-      <c r="AJ3" s="639" t="s">
+      <c r="AI3" s="647"/>
+      <c r="AJ3" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="AK3" s="638"/>
-      <c r="AL3" s="637" t="s">
+      <c r="AK3" s="647"/>
+      <c r="AL3" s="648" t="s">
         <v>66</v>
       </c>
-      <c r="AM3" s="638"/>
+      <c r="AM3" s="647"/>
     </row>
     <row r="4" spans="1:39" s="127" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="644"/>
-      <c r="B4" s="647"/>
-      <c r="C4" s="648"/>
+      <c r="A4" s="635"/>
+      <c r="B4" s="638"/>
+      <c r="C4" s="639"/>
       <c r="D4" s="265">
         <v>2030</v>
       </c>
@@ -29528,7 +29548,7 @@
       <c r="I4" s="266">
         <v>2040</v>
       </c>
-      <c r="K4" s="644"/>
+      <c r="K4" s="635"/>
       <c r="L4" s="642"/>
       <c r="M4" s="643"/>
       <c r="N4" s="265">
@@ -29549,7 +29569,7 @@
       <c r="S4" s="266">
         <v>2040</v>
       </c>
-      <c r="U4" s="644"/>
+      <c r="U4" s="635"/>
       <c r="V4" s="642"/>
       <c r="W4" s="643"/>
       <c r="X4" s="265">
@@ -29570,7 +29590,7 @@
       <c r="AC4" s="266">
         <v>2040</v>
       </c>
-      <c r="AE4" s="644"/>
+      <c r="AE4" s="635"/>
       <c r="AF4" s="642"/>
       <c r="AG4" s="643"/>
       <c r="AH4" s="265">
@@ -29633,7 +29653,7 @@
       <c r="AM5" s="201"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="634" t="s">
+      <c r="A6" s="644" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="135" t="s">
@@ -29666,7 +29686,7 @@
         <f>Indata!I32</f>
         <v>21.293751803814949</v>
       </c>
-      <c r="K6" s="634" t="s">
+      <c r="K6" s="644" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="135" t="s">
@@ -29699,7 +29719,7 @@
         <f>'Modell - Drivmedelpriser'!J24</f>
         <v>27.329509698551796</v>
       </c>
-      <c r="U6" s="634" t="s">
+      <c r="U6" s="644" t="s">
         <v>0</v>
       </c>
       <c r="V6" s="135" t="s">
@@ -29732,7 +29752,7 @@
         <f t="shared" ref="AC6:AC8" si="4">S6</f>
         <v>27.329509698551796</v>
       </c>
-      <c r="AE6" s="634" t="s">
+      <c r="AE6" s="644" t="s">
         <v>0</v>
       </c>
       <c r="AF6" s="135" t="s">
@@ -29767,7 +29787,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="635"/>
+      <c r="A7" s="645"/>
       <c r="B7" s="136" t="s">
         <v>9</v>
       </c>
@@ -29798,7 +29818,7 @@
         <f>Indata!I33</f>
         <v>22.557131724953557</v>
       </c>
-      <c r="K7" s="635"/>
+      <c r="K7" s="645"/>
       <c r="L7" s="136" t="s">
         <v>9</v>
       </c>
@@ -29829,7 +29849,7 @@
         <f>'Modell - Drivmedelpriser'!J43</f>
         <v>24.89327119863777</v>
       </c>
-      <c r="U7" s="635"/>
+      <c r="U7" s="645"/>
       <c r="V7" s="136" t="s">
         <v>9</v>
       </c>
@@ -29860,7 +29880,7 @@
         <f t="shared" si="4"/>
         <v>24.89327119863777</v>
       </c>
-      <c r="AE7" s="635"/>
+      <c r="AE7" s="645"/>
       <c r="AF7" s="136" t="s">
         <v>9</v>
       </c>
@@ -29893,7 +29913,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="635"/>
+      <c r="A8" s="645"/>
       <c r="B8" s="136" t="s">
         <v>7</v>
       </c>
@@ -29924,7 +29944,7 @@
         <f>Indata!I34</f>
         <v>4.1598749999999995</v>
       </c>
-      <c r="K8" s="635"/>
+      <c r="K8" s="645"/>
       <c r="L8" s="136" t="s">
         <v>7</v>
       </c>
@@ -29955,7 +29975,7 @@
         <f>'Modell - Drivmedelpriser'!J75</f>
         <v>4.1598749999999995</v>
       </c>
-      <c r="U8" s="635"/>
+      <c r="U8" s="645"/>
       <c r="V8" s="136" t="s">
         <v>7</v>
       </c>
@@ -29986,7 +30006,7 @@
         <f t="shared" si="4"/>
         <v>4.1598749999999995</v>
       </c>
-      <c r="AE8" s="635"/>
+      <c r="AE8" s="645"/>
       <c r="AF8" s="136" t="s">
         <v>7</v>
       </c>
@@ -30019,7 +30039,7 @@
       </c>
     </row>
     <row r="9" spans="1:39" s="303" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="635"/>
+      <c r="A9" s="645"/>
       <c r="B9" s="187" t="s">
         <v>20</v>
       </c>
@@ -30050,7 +30070,7 @@
         <f>Indata!I35</f>
         <v>21.888963239913203</v>
       </c>
-      <c r="K9" s="635"/>
+      <c r="K9" s="645"/>
       <c r="L9" s="187" t="s">
         <v>20</v>
       </c>
@@ -30081,7 +30101,7 @@
         <f t="shared" si="12"/>
         <v>26.181733806320725</v>
       </c>
-      <c r="U9" s="635"/>
+      <c r="U9" s="645"/>
       <c r="V9" s="187" t="s">
         <v>20</v>
       </c>
@@ -30112,7 +30132,7 @@
         <f t="shared" si="13"/>
         <v>26.181733806320722</v>
       </c>
-      <c r="AE9" s="635"/>
+      <c r="AE9" s="645"/>
       <c r="AF9" s="187" t="s">
         <v>20</v>
       </c>
@@ -30145,7 +30165,7 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="636"/>
+      <c r="A10" s="646"/>
       <c r="B10" s="188" t="s">
         <v>234</v>
       </c>
@@ -30170,7 +30190,7 @@
       <c r="I10" s="225" t="s">
         <v>78</v>
       </c>
-      <c r="K10" s="636"/>
+      <c r="K10" s="646"/>
       <c r="L10" s="188" t="s">
         <v>234</v>
       </c>
@@ -30201,7 +30221,7 @@
         <f t="shared" si="15"/>
         <v>0.1961157556599078</v>
       </c>
-      <c r="U10" s="636"/>
+      <c r="U10" s="646"/>
       <c r="V10" s="188" t="s">
         <v>234</v>
       </c>
@@ -30232,7 +30252,7 @@
         <f t="shared" si="16"/>
         <v>0.1961157556599078</v>
       </c>
-      <c r="AE10" s="636"/>
+      <c r="AE10" s="646"/>
       <c r="AF10" s="188" t="s">
         <v>234</v>
       </c>
@@ -30334,7 +30354,7 @@
       <c r="AM12" s="201"/>
     </row>
     <row r="13" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="634" t="s">
+      <c r="A13" s="644" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="135" t="s">
@@ -30367,7 +30387,7 @@
         <f>Indata!I29</f>
         <v>0.49219920755019081</v>
       </c>
-      <c r="K13" s="634" t="s">
+      <c r="K13" s="644" t="s">
         <v>38</v>
       </c>
       <c r="L13" s="135" t="s">
@@ -30400,7 +30420,7 @@
         <f>I13*(100%+S$10*'Indata - Effektsamband-Faktorer'!$E$5)*(1-Indata!I$19)</f>
         <v>0.48737280657399518</v>
       </c>
-      <c r="U13" s="634" t="s">
+      <c r="U13" s="644" t="s">
         <v>38</v>
       </c>
       <c r="V13" s="135" t="s">
@@ -30433,7 +30453,7 @@
         <f t="shared" ref="AC13:AC15" si="22">S13</f>
         <v>0.48737280657399518</v>
       </c>
-      <c r="AE13" s="634" t="s">
+      <c r="AE13" s="644" t="s">
         <v>38</v>
       </c>
       <c r="AF13" s="135" t="s">
@@ -30468,7 +30488,7 @@
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="635"/>
+      <c r="A14" s="645"/>
       <c r="B14" s="136" t="s">
         <v>9</v>
       </c>
@@ -30499,7 +30519,7 @@
         <f>Indata!I30</f>
         <v>0.49160078067679608</v>
       </c>
-      <c r="K14" s="635"/>
+      <c r="K14" s="645"/>
       <c r="L14" s="136" t="s">
         <v>9</v>
       </c>
@@ -30530,7 +30550,7 @@
         <f>I14*(100%+S$10*'Indata - Effektsamband-Faktorer'!$E$5)*(1-Indata!I$19)</f>
         <v>0.4867802477475246</v>
       </c>
-      <c r="U14" s="635"/>
+      <c r="U14" s="645"/>
       <c r="V14" s="136" t="s">
         <v>9</v>
       </c>
@@ -30561,7 +30581,7 @@
         <f t="shared" si="22"/>
         <v>0.4867802477475246</v>
       </c>
-      <c r="AE14" s="635"/>
+      <c r="AE14" s="645"/>
       <c r="AF14" s="136" t="s">
         <v>9</v>
       </c>
@@ -30594,7 +30614,7 @@
       </c>
     </row>
     <row r="15" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="636"/>
+      <c r="A15" s="646"/>
       <c r="B15" s="137" t="s">
         <v>7</v>
       </c>
@@ -30625,7 +30645,7 @@
         <f>Indata!I31</f>
         <v>1.6150000000000002</v>
       </c>
-      <c r="K15" s="636"/>
+      <c r="K15" s="646"/>
       <c r="L15" s="137" t="s">
         <v>7</v>
       </c>
@@ -30656,7 +30676,7 @@
         <f>I15*(1-Indata!I$19)</f>
         <v>1.6150000000000002</v>
       </c>
-      <c r="U15" s="636"/>
+      <c r="U15" s="646"/>
       <c r="V15" s="137" t="s">
         <v>7</v>
       </c>
@@ -30687,7 +30707,7 @@
         <f t="shared" si="22"/>
         <v>1.6150000000000002</v>
       </c>
-      <c r="AE15" s="636"/>
+      <c r="AE15" s="646"/>
       <c r="AF15" s="137" t="s">
         <v>7</v>
       </c>
@@ -31370,7 +31390,7 @@
       <c r="AM23" s="201"/>
     </row>
     <row r="24" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="634" t="s">
+      <c r="A24" s="644" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="135" t="s">
@@ -31403,7 +31423,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K24" s="634" t="s">
+      <c r="K24" s="644" t="s">
         <v>21</v>
       </c>
       <c r="L24" s="135" t="s">
@@ -31436,7 +31456,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="U24" s="634" t="s">
+      <c r="U24" s="644" t="s">
         <v>21</v>
       </c>
       <c r="V24" s="135" t="s">
@@ -31469,7 +31489,7 @@
         <f t="shared" ref="AC24:AC26" si="50">S24</f>
         <v>0</v>
       </c>
-      <c r="AE24" s="634" t="s">
+      <c r="AE24" s="644" t="s">
         <v>21</v>
       </c>
       <c r="AF24" s="135" t="s">
@@ -31504,7 +31524,7 @@
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A25" s="635"/>
+      <c r="A25" s="645"/>
       <c r="B25" s="136" t="s">
         <v>9</v>
       </c>
@@ -31535,7 +31555,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K25" s="635"/>
+      <c r="K25" s="645"/>
       <c r="L25" s="136" t="s">
         <v>9</v>
       </c>
@@ -31566,7 +31586,7 @@
         <f t="shared" ref="S25:S26" si="61">I25</f>
         <v>0</v>
       </c>
-      <c r="U25" s="635"/>
+      <c r="U25" s="645"/>
       <c r="V25" s="136" t="s">
         <v>9</v>
       </c>
@@ -31597,7 +31617,7 @@
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AE25" s="635"/>
+      <c r="AE25" s="645"/>
       <c r="AF25" s="136" t="s">
         <v>9</v>
       </c>
@@ -31630,7 +31650,7 @@
       </c>
     </row>
     <row r="26" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="636"/>
+      <c r="A26" s="646"/>
       <c r="B26" s="137" t="s">
         <v>7</v>
       </c>
@@ -31661,7 +31681,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K26" s="636"/>
+      <c r="K26" s="646"/>
       <c r="L26" s="137" t="s">
         <v>7</v>
       </c>
@@ -31692,7 +31712,7 @@
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="U26" s="636"/>
+      <c r="U26" s="646"/>
       <c r="V26" s="137" t="s">
         <v>7</v>
       </c>
@@ -31723,7 +31743,7 @@
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AE26" s="636"/>
+      <c r="AE26" s="646"/>
       <c r="AF26" s="137" t="s">
         <v>7</v>
       </c>
@@ -31831,7 +31851,7 @@
       <c r="AM28" s="201"/>
     </row>
     <row r="29" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="634" t="s">
+      <c r="A29" s="644" t="s">
         <v>75</v>
       </c>
       <c r="B29" s="135" t="s">
@@ -31864,7 +31884,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K29" s="634" t="s">
+      <c r="K29" s="644" t="s">
         <v>75</v>
       </c>
       <c r="L29" s="135" t="s">
@@ -31897,7 +31917,7 @@
         <f t="shared" ref="S29:S31" si="68">I29</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="U29" s="634" t="s">
+      <c r="U29" s="644" t="s">
         <v>75</v>
       </c>
       <c r="V29" s="135" t="s">
@@ -31930,7 +31950,7 @@
         <f t="shared" ref="AC29:AC31" si="73">S29</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE29" s="634" t="s">
+      <c r="AE29" s="644" t="s">
         <v>75</v>
       </c>
       <c r="AF29" s="135" t="s">
@@ -31965,7 +31985,7 @@
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A30" s="635"/>
+      <c r="A30" s="645"/>
       <c r="B30" s="136" t="s">
         <v>9</v>
       </c>
@@ -31996,7 +32016,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K30" s="635"/>
+      <c r="K30" s="645"/>
       <c r="L30" s="136" t="s">
         <v>9</v>
       </c>
@@ -32027,7 +32047,7 @@
         <f t="shared" si="68"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="U30" s="635"/>
+      <c r="U30" s="645"/>
       <c r="V30" s="136" t="s">
         <v>9</v>
       </c>
@@ -32058,7 +32078,7 @@
         <f t="shared" si="73"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE30" s="635"/>
+      <c r="AE30" s="645"/>
       <c r="AF30" s="136" t="s">
         <v>9</v>
       </c>
@@ -32091,7 +32111,7 @@
       </c>
     </row>
     <row r="31" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="636"/>
+      <c r="A31" s="646"/>
       <c r="B31" s="137" t="s">
         <v>7</v>
       </c>
@@ -32122,7 +32142,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K31" s="636"/>
+      <c r="K31" s="646"/>
       <c r="L31" s="137" t="s">
         <v>7</v>
       </c>
@@ -32153,7 +32173,7 @@
         <f t="shared" si="68"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="U31" s="636"/>
+      <c r="U31" s="646"/>
       <c r="V31" s="137" t="s">
         <v>7</v>
       </c>
@@ -32184,7 +32204,7 @@
         <f t="shared" si="73"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE31" s="636"/>
+      <c r="AE31" s="646"/>
       <c r="AF31" s="137" t="s">
         <v>7</v>
       </c>
@@ -32875,7 +32895,7 @@
       <c r="AM39" s="201"/>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A40" s="634" t="s">
+      <c r="A40" s="644" t="s">
         <v>77</v>
       </c>
       <c r="B40" s="135" t="s">
@@ -32908,7 +32928,7 @@
         <f t="shared" si="90"/>
         <v>20.490767763608162</v>
       </c>
-      <c r="K40" s="634" t="s">
+      <c r="K40" s="644" t="s">
         <v>77</v>
       </c>
       <c r="L40" s="135" t="s">
@@ -32941,7 +32961,7 @@
         <f t="shared" si="91"/>
         <v>23.329659844074406</v>
       </c>
-      <c r="U40" s="634" t="s">
+      <c r="U40" s="644" t="s">
         <v>77</v>
       </c>
       <c r="V40" s="135" t="s">
@@ -32974,7 +32994,7 @@
         <f t="shared" ref="AC40:AC42" si="96">S40</f>
         <v>23.329659844074406</v>
       </c>
-      <c r="AE40" s="634" t="s">
+      <c r="AE40" s="644" t="s">
         <v>77</v>
       </c>
       <c r="AF40" s="135" t="s">
@@ -33009,7 +33029,7 @@
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A41" s="635"/>
+      <c r="A41" s="645"/>
       <c r="B41" s="136" t="s">
         <v>9</v>
       </c>
@@ -33040,7 +33060,7 @@
         <f t="shared" si="90"/>
         <v>21.099103565816492</v>
       </c>
-      <c r="K41" s="635"/>
+      <c r="K41" s="645"/>
       <c r="L41" s="136" t="s">
         <v>9</v>
       </c>
@@ -33071,7 +33091,7 @@
         <f t="shared" si="91"/>
         <v>22.127552721319212</v>
       </c>
-      <c r="U41" s="635"/>
+      <c r="U41" s="645"/>
       <c r="V41" s="136" t="s">
         <v>9</v>
       </c>
@@ -33102,7 +33122,7 @@
         <f t="shared" si="96"/>
         <v>22.127552721319212</v>
       </c>
-      <c r="AE41" s="635"/>
+      <c r="AE41" s="645"/>
       <c r="AF41" s="136" t="s">
         <v>9</v>
       </c>
@@ -33135,7 +33155,7 @@
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A42" s="635"/>
+      <c r="A42" s="645"/>
       <c r="B42" s="136" t="s">
         <v>7</v>
       </c>
@@ -33166,7 +33186,7 @@
         <f t="shared" si="90"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="K42" s="635"/>
+      <c r="K42" s="645"/>
       <c r="L42" s="136" t="s">
         <v>7</v>
       </c>
@@ -33197,7 +33217,7 @@
         <f t="shared" si="91"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="U42" s="635"/>
+      <c r="U42" s="645"/>
       <c r="V42" s="136" t="s">
         <v>7</v>
       </c>
@@ -33228,7 +33248,7 @@
         <f t="shared" si="96"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="AE42" s="635"/>
+      <c r="AE42" s="645"/>
       <c r="AF42" s="136" t="s">
         <v>7</v>
       </c>
@@ -33261,7 +33281,7 @@
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A43" s="635"/>
+      <c r="A43" s="645"/>
       <c r="B43" s="187" t="s">
         <v>76</v>
       </c>
@@ -33290,7 +33310,7 @@
         <f t="shared" si="104"/>
         <v>18.064425082921922</v>
       </c>
-      <c r="K43" s="635"/>
+      <c r="K43" s="645"/>
       <c r="L43" s="187" t="s">
         <v>76</v>
       </c>
@@ -33321,7 +33341,7 @@
         <f t="shared" ref="S43" si="105">SUMPRODUCT(S40:S42,S34:S36)/S37</f>
         <v>18.645576333860959</v>
       </c>
-      <c r="U43" s="635"/>
+      <c r="U43" s="645"/>
       <c r="V43" s="187" t="s">
         <v>76</v>
       </c>
@@ -33352,7 +33372,7 @@
         <f t="shared" si="106"/>
         <v>18.645576333860962</v>
       </c>
-      <c r="AE43" s="635"/>
+      <c r="AE43" s="645"/>
       <c r="AF43" s="187" t="s">
         <v>76</v>
       </c>
@@ -33385,7 +33405,7 @@
       </c>
     </row>
     <row r="44" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="636"/>
+      <c r="A44" s="646"/>
       <c r="B44" s="188" t="s">
         <v>234</v>
       </c>
@@ -33410,7 +33430,7 @@
       <c r="I44" s="225" t="s">
         <v>78</v>
       </c>
-      <c r="K44" s="636"/>
+      <c r="K44" s="646"/>
       <c r="L44" s="188" t="s">
         <v>234</v>
       </c>
@@ -33441,7 +33461,7 @@
         <f>S43/E43-1</f>
         <v>-5.1358020489668088E-2</v>
       </c>
-      <c r="U44" s="636"/>
+      <c r="U44" s="646"/>
       <c r="V44" s="188" t="s">
         <v>234</v>
       </c>
@@ -33472,7 +33492,7 @@
         <f>AC43/E43-1</f>
         <v>-5.1358020489667866E-2</v>
       </c>
-      <c r="AE44" s="636"/>
+      <c r="AE44" s="646"/>
       <c r="AF44" s="188" t="s">
         <v>234</v>
       </c>
@@ -33580,7 +33600,7 @@
       <c r="AM46" s="78"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A47" s="634" t="s">
+      <c r="A47" s="644" t="s">
         <v>29</v>
       </c>
       <c r="B47" s="135" t="s">
@@ -33613,7 +33633,7 @@
         <f>Indata!I39</f>
         <v>11648700</v>
       </c>
-      <c r="K47" s="634" t="s">
+      <c r="K47" s="644" t="s">
         <v>29</v>
       </c>
       <c r="L47" s="135" t="s">
@@ -33646,7 +33666,7 @@
         <f t="shared" si="107"/>
         <v>11648700</v>
       </c>
-      <c r="U47" s="634" t="s">
+      <c r="U47" s="644" t="s">
         <v>29</v>
       </c>
       <c r="V47" s="135" t="s">
@@ -33679,7 +33699,7 @@
         <f t="shared" ref="AC47:AC49" si="112">S47</f>
         <v>11648700</v>
       </c>
-      <c r="AE47" s="634" t="s">
+      <c r="AE47" s="644" t="s">
         <v>29</v>
       </c>
       <c r="AF47" s="135" t="s">
@@ -33714,7 +33734,7 @@
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A48" s="635"/>
+      <c r="A48" s="645"/>
       <c r="B48" s="136" t="s">
         <v>29</v>
       </c>
@@ -33745,7 +33765,7 @@
         <f>Indata!I40</f>
         <v>0.52928701904391762</v>
       </c>
-      <c r="K48" s="635"/>
+      <c r="K48" s="645"/>
       <c r="L48" s="136" t="s">
         <v>29</v>
       </c>
@@ -33776,7 +33796,7 @@
         <f>(1+'Indata - Effektsamband-Faktorer'!$E$7*S44)*'Modell - Lätta fordon'!I48</f>
         <v>0.53200533240081493</v>
       </c>
-      <c r="U48" s="635"/>
+      <c r="U48" s="645"/>
       <c r="V48" s="136" t="s">
         <v>29</v>
       </c>
@@ -33807,7 +33827,7 @@
         <f t="shared" si="112"/>
         <v>0.53200533240081493</v>
       </c>
-      <c r="AE48" s="635"/>
+      <c r="AE48" s="645"/>
       <c r="AF48" s="136" t="s">
         <v>29</v>
       </c>
@@ -33840,7 +33860,7 @@
       </c>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A49" s="635"/>
+      <c r="A49" s="645"/>
       <c r="B49" s="136" t="s">
         <v>34</v>
       </c>
@@ -33871,7 +33891,7 @@
         <f t="shared" si="118"/>
         <v>6165505.6987368828</v>
       </c>
-      <c r="K49" s="635"/>
+      <c r="K49" s="645"/>
       <c r="L49" s="136" t="s">
         <v>34</v>
       </c>
@@ -33902,7 +33922,7 @@
         <f t="shared" ref="S49" si="121">S47*S48</f>
         <v>6197170.5155373728</v>
       </c>
-      <c r="U49" s="635"/>
+      <c r="U49" s="645"/>
       <c r="V49" s="136" t="s">
         <v>34</v>
       </c>
@@ -33933,7 +33953,7 @@
         <f t="shared" si="112"/>
         <v>6197170.5155373728</v>
       </c>
-      <c r="AE49" s="635"/>
+      <c r="AE49" s="645"/>
       <c r="AF49" s="136" t="s">
         <v>34</v>
       </c>
@@ -33966,7 +33986,7 @@
       </c>
     </row>
     <row r="50" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="636"/>
+      <c r="A50" s="646"/>
       <c r="B50" s="188" t="s">
         <v>234</v>
       </c>
@@ -33991,7 +34011,7 @@
       <c r="I50" s="225" t="s">
         <v>78</v>
       </c>
-      <c r="K50" s="636"/>
+      <c r="K50" s="646"/>
       <c r="L50" s="188" t="s">
         <v>234</v>
       </c>
@@ -34022,7 +34042,7 @@
         <f>S49/E49-1</f>
         <v>5.1358020489669087E-3</v>
       </c>
-      <c r="U50" s="636"/>
+      <c r="U50" s="646"/>
       <c r="V50" s="188" t="s">
         <v>234</v>
       </c>
@@ -34053,7 +34073,7 @@
         <f>AC49/E49-1</f>
         <v>5.1358020489669087E-3</v>
       </c>
-      <c r="AE50" s="636"/>
+      <c r="AE50" s="646"/>
       <c r="AF50" s="188" t="s">
         <v>234</v>
       </c>
@@ -35617,6 +35637,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="AE57:AE60"/>
+    <mergeCell ref="AE61:AE64"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="U18:U21"/>
+    <mergeCell ref="U24:U26"/>
+    <mergeCell ref="U29:U31"/>
+    <mergeCell ref="U34:U37"/>
+    <mergeCell ref="U40:U44"/>
+    <mergeCell ref="U47:U50"/>
+    <mergeCell ref="AE34:AE37"/>
+    <mergeCell ref="AE40:AE44"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="K47:K50"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="K29:K31"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="U6:U10"/>
+    <mergeCell ref="U13:U15"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AE6:AE10"/>
+    <mergeCell ref="AE13:AE15"/>
+    <mergeCell ref="AF3:AG4"/>
     <mergeCell ref="AE86:AE89"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C4"/>
@@ -35633,48 +35695,6 @@
     <mergeCell ref="AE24:AE26"/>
     <mergeCell ref="AE29:AE31"/>
     <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AE6:AE10"/>
-    <mergeCell ref="AE13:AE15"/>
-    <mergeCell ref="AF3:AG4"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="U6:U10"/>
-    <mergeCell ref="U13:U15"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="K47:K50"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="K40:K44"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="K34:K37"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="K29:K31"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="AE57:AE60"/>
-    <mergeCell ref="AE61:AE64"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="U18:U21"/>
-    <mergeCell ref="U24:U26"/>
-    <mergeCell ref="U29:U31"/>
-    <mergeCell ref="U34:U37"/>
-    <mergeCell ref="U40:U44"/>
-    <mergeCell ref="U47:U50"/>
-    <mergeCell ref="AE34:AE37"/>
-    <mergeCell ref="AE40:AE44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Many updates, including scripts for directed and robust search
</commit_message>
<xml_diff>
--- a/models/trv_scenario2.xlsx
+++ b/models/trv_scenario2.xlsx
@@ -1282,7 +1282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1709" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="410">
   <si>
     <t>Drivmedelspris</t>
   </si>
@@ -2628,6 +2628,15 @@
   </si>
   <si>
     <t>Förändring i utsläpp bilar</t>
+  </si>
+  <si>
+    <t>Andel elenergi</t>
+  </si>
+  <si>
+    <t>Driving cost light veh comp. Reference</t>
+  </si>
+  <si>
+    <t>Driving cost truck comp. Reference</t>
   </si>
 </sst>
 </file>
@@ -18558,10 +18567,10 @@
   <dimension ref="A1:S81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="E76" sqref="E76"/>
+      <selection pane="bottomRight" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21067,6 +21076,33 @@
       <c r="D74" s="40">
         <f>Resultat!F37/'Indata - Utsläpp'!B15-1</f>
         <v>-0.73481851843620594</v>
+      </c>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C75" s="40" t="s">
+        <v>407</v>
+      </c>
+      <c r="D75" s="40">
+        <f>D73/D70</f>
+        <v>0.11067922200266737</v>
+      </c>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C76" s="40" t="s">
+        <v>408</v>
+      </c>
+      <c r="D76" s="40">
+        <f>Resultat!F23/Resultat!D23</f>
+        <v>2.6929197009211712</v>
+      </c>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C77" s="40" t="s">
+        <v>409</v>
+      </c>
+      <c r="D77" s="40">
+        <f>Resultat!F26/Resultat!D26</f>
+        <v>1.9499962263346504</v>
       </c>
     </row>
     <row r="78" spans="2:9" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -21165,7 +21201,7 @@
   <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="6" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
       <selection pane="bottomRight" activeCell="F37" sqref="F37"/>

</xml_diff>

<commit_message>
Towards paper ready analysis see description
Re-naming of scripts
Separation of open exploration (OE) analysis script for manual and sampled policies
Various improvements for manual policies OE script, including color palette for polices
New runs
+ many misc
</commit_message>
<xml_diff>
--- a/models/trv_scenario2.xlsx
+++ b/models/trv_scenario2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Beskrivning" sheetId="19" r:id="rId1"/>
@@ -45,7 +45,7 @@
     <definedName name="kr_till_öre">'[1]Koefficienter &amp; omvandlingstal'!$A$20</definedName>
     <definedName name="m3_till_liter">'[1]Koefficienter &amp; omvandlingstal'!$A$21</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="autoNoTable" calcOnSave="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1282,7 +1282,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1712" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="411">
   <si>
     <t>Drivmedelspris</t>
   </si>
@@ -2637,6 +2637,9 @@
   </si>
   <si>
     <t>Driving cost truck comp. Reference</t>
+  </si>
+  <si>
+    <t>Konsumentöverskott (delta) beräknat m.h.a "rule of half"</t>
   </si>
 </sst>
 </file>
@@ -5263,6 +5266,39 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5278,44 +5314,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5323,30 +5350,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5359,45 +5362,45 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5407,6 +5410,36 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="22" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5416,41 +5449,11 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="28">
@@ -10590,87 +10593,87 @@
     </row>
     <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:39" s="325" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="643" t="s">
+      <c r="A3" s="638" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="649" t="s">
+      <c r="B3" s="640" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="650"/>
-      <c r="D3" s="643" t="s">
+      <c r="C3" s="641"/>
+      <c r="D3" s="638" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="642"/>
-      <c r="F3" s="643" t="s">
+      <c r="E3" s="651"/>
+      <c r="F3" s="638" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="642"/>
-      <c r="H3" s="641" t="s">
+      <c r="G3" s="651"/>
+      <c r="H3" s="652" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="642"/>
-      <c r="K3" s="643" t="s">
+      <c r="I3" s="651"/>
+      <c r="K3" s="638" t="s">
         <v>67</v>
       </c>
-      <c r="L3" s="649" t="s">
+      <c r="L3" s="640" t="s">
         <v>240</v>
       </c>
-      <c r="M3" s="650"/>
-      <c r="N3" s="643" t="s">
+      <c r="M3" s="641"/>
+      <c r="N3" s="638" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="642"/>
-      <c r="P3" s="643" t="s">
+      <c r="O3" s="651"/>
+      <c r="P3" s="638" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="642"/>
-      <c r="R3" s="641" t="s">
+      <c r="Q3" s="651"/>
+      <c r="R3" s="652" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="642"/>
-      <c r="U3" s="643" t="s">
+      <c r="S3" s="651"/>
+      <c r="U3" s="638" t="s">
         <v>67</v>
       </c>
-      <c r="V3" s="649" t="s">
+      <c r="V3" s="640" t="s">
         <v>241</v>
       </c>
-      <c r="W3" s="650"/>
-      <c r="X3" s="643" t="s">
+      <c r="W3" s="641"/>
+      <c r="X3" s="638" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="642"/>
-      <c r="Z3" s="643" t="s">
+      <c r="Y3" s="651"/>
+      <c r="Z3" s="638" t="s">
         <v>65</v>
       </c>
-      <c r="AA3" s="642"/>
-      <c r="AB3" s="641" t="s">
+      <c r="AA3" s="651"/>
+      <c r="AB3" s="652" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="642"/>
-      <c r="AE3" s="643" t="s">
+      <c r="AC3" s="651"/>
+      <c r="AE3" s="638" t="s">
         <v>67</v>
       </c>
-      <c r="AF3" s="649" t="s">
+      <c r="AF3" s="640" t="s">
         <v>238</v>
       </c>
-      <c r="AG3" s="650"/>
-      <c r="AH3" s="643" t="s">
+      <c r="AG3" s="641"/>
+      <c r="AH3" s="638" t="s">
         <v>64</v>
       </c>
-      <c r="AI3" s="642"/>
-      <c r="AJ3" s="643" t="s">
+      <c r="AI3" s="651"/>
+      <c r="AJ3" s="638" t="s">
         <v>65</v>
       </c>
-      <c r="AK3" s="642"/>
-      <c r="AL3" s="641" t="s">
+      <c r="AK3" s="651"/>
+      <c r="AL3" s="652" t="s">
         <v>66</v>
       </c>
-      <c r="AM3" s="642"/>
+      <c r="AM3" s="651"/>
     </row>
     <row r="4" spans="1:39" s="127" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="648"/>
-      <c r="B4" s="651"/>
-      <c r="C4" s="652"/>
+      <c r="A4" s="639"/>
+      <c r="B4" s="642"/>
+      <c r="C4" s="643"/>
       <c r="D4" s="265">
         <v>2030</v>
       </c>
@@ -10689,9 +10692,9 @@
       <c r="I4" s="266">
         <v>2040</v>
       </c>
-      <c r="K4" s="648"/>
-      <c r="L4" s="651"/>
-      <c r="M4" s="652"/>
+      <c r="K4" s="639"/>
+      <c r="L4" s="642"/>
+      <c r="M4" s="643"/>
       <c r="N4" s="265">
         <v>2030</v>
       </c>
@@ -10710,9 +10713,9 @@
       <c r="S4" s="266">
         <v>2040</v>
       </c>
-      <c r="U4" s="648"/>
-      <c r="V4" s="651"/>
-      <c r="W4" s="652"/>
+      <c r="U4" s="639"/>
+      <c r="V4" s="642"/>
+      <c r="W4" s="643"/>
       <c r="X4" s="265">
         <v>2030</v>
       </c>
@@ -10731,9 +10734,9 @@
       <c r="AC4" s="266">
         <v>2040</v>
       </c>
-      <c r="AE4" s="648"/>
-      <c r="AF4" s="651"/>
-      <c r="AG4" s="652"/>
+      <c r="AE4" s="639"/>
+      <c r="AF4" s="642"/>
+      <c r="AG4" s="643"/>
       <c r="AH4" s="265">
         <v>2030</v>
       </c>
@@ -10794,7 +10797,7 @@
       <c r="AM5" s="76"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="638" t="s">
+      <c r="A6" s="648" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="135" t="s">
@@ -10827,7 +10830,7 @@
         <f>Indata!I54</f>
         <v>19.161594511883557</v>
       </c>
-      <c r="K6" s="638" t="s">
+      <c r="K6" s="648" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="135" t="s">
@@ -10860,7 +10863,7 @@
         <f>'Modell - Drivmedelpriser'!J58</f>
         <v>19.161594511883557</v>
       </c>
-      <c r="U6" s="638" t="s">
+      <c r="U6" s="648" t="s">
         <v>0</v>
       </c>
       <c r="V6" s="135" t="s">
@@ -10893,7 +10896,7 @@
         <f t="shared" ref="AC6:AC7" si="4">S6</f>
         <v>19.161594511883557</v>
       </c>
-      <c r="AE6" s="638" t="s">
+      <c r="AE6" s="648" t="s">
         <v>0</v>
       </c>
       <c r="AF6" s="135" t="s">
@@ -10928,7 +10931,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="639"/>
+      <c r="A7" s="649"/>
       <c r="B7" s="136" t="s">
         <v>7</v>
       </c>
@@ -10959,7 +10962,7 @@
         <f>Indata!I55</f>
         <v>1.4034</v>
       </c>
-      <c r="K7" s="639"/>
+      <c r="K7" s="649"/>
       <c r="L7" s="136" t="s">
         <v>7</v>
       </c>
@@ -10990,7 +10993,7 @@
         <f>'Modell - Drivmedelpriser'!J84</f>
         <v>1.4034</v>
       </c>
-      <c r="U7" s="639"/>
+      <c r="U7" s="649"/>
       <c r="V7" s="136" t="s">
         <v>7</v>
       </c>
@@ -11021,7 +11024,7 @@
         <f t="shared" si="4"/>
         <v>1.4034</v>
       </c>
-      <c r="AE7" s="639"/>
+      <c r="AE7" s="649"/>
       <c r="AF7" s="136" t="s">
         <v>7</v>
       </c>
@@ -11054,7 +11057,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="640"/>
+      <c r="A8" s="650"/>
       <c r="B8" s="188" t="s">
         <v>244</v>
       </c>
@@ -11079,7 +11082,7 @@
       <c r="I8" s="287" t="s">
         <v>78</v>
       </c>
-      <c r="K8" s="640"/>
+      <c r="K8" s="650"/>
       <c r="L8" s="188" t="s">
         <v>244</v>
       </c>
@@ -11110,7 +11113,7 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="U8" s="640"/>
+      <c r="U8" s="650"/>
       <c r="V8" s="188" t="s">
         <v>244</v>
       </c>
@@ -11141,7 +11144,7 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AE8" s="640"/>
+      <c r="AE8" s="650"/>
       <c r="AF8" s="188" t="s">
         <v>244</v>
       </c>
@@ -13143,7 +13146,7 @@
       <c r="AM28" s="77"/>
     </row>
     <row r="29" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="638" t="s">
+      <c r="A29" s="648" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="135" t="s">
@@ -13176,7 +13179,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K29" s="638" t="s">
+      <c r="K29" s="648" t="s">
         <v>21</v>
       </c>
       <c r="L29" s="135" t="s">
@@ -13209,7 +13212,7 @@
         <f t="shared" ref="S29:S32" si="65">I29</f>
         <v>0</v>
       </c>
-      <c r="U29" s="638" t="s">
+      <c r="U29" s="648" t="s">
         <v>21</v>
       </c>
       <c r="V29" s="135" t="s">
@@ -13242,7 +13245,7 @@
         <f t="shared" ref="AC29:AC32" si="70">S29</f>
         <v>0</v>
       </c>
-      <c r="AE29" s="638" t="s">
+      <c r="AE29" s="648" t="s">
         <v>21</v>
       </c>
       <c r="AF29" s="135" t="s">
@@ -13277,7 +13280,7 @@
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A30" s="639"/>
+      <c r="A30" s="649"/>
       <c r="B30" s="136" t="s">
         <v>117</v>
       </c>
@@ -13308,7 +13311,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K30" s="639"/>
+      <c r="K30" s="649"/>
       <c r="L30" s="136" t="s">
         <v>117</v>
       </c>
@@ -13339,7 +13342,7 @@
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
-      <c r="U30" s="639"/>
+      <c r="U30" s="649"/>
       <c r="V30" s="136" t="s">
         <v>117</v>
       </c>
@@ -13370,7 +13373,7 @@
         <f t="shared" si="70"/>
         <v>0</v>
       </c>
-      <c r="AE30" s="639"/>
+      <c r="AE30" s="649"/>
       <c r="AF30" s="136" t="s">
         <v>117</v>
       </c>
@@ -13403,7 +13406,7 @@
       </c>
     </row>
     <row r="31" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A31" s="639"/>
+      <c r="A31" s="649"/>
       <c r="B31" s="136" t="s">
         <v>118</v>
       </c>
@@ -13434,7 +13437,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K31" s="639"/>
+      <c r="K31" s="649"/>
       <c r="L31" s="136" t="s">
         <v>118</v>
       </c>
@@ -13465,7 +13468,7 @@
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
-      <c r="U31" s="639"/>
+      <c r="U31" s="649"/>
       <c r="V31" s="136" t="s">
         <v>118</v>
       </c>
@@ -13496,7 +13499,7 @@
         <f t="shared" si="70"/>
         <v>0</v>
       </c>
-      <c r="AE31" s="639"/>
+      <c r="AE31" s="649"/>
       <c r="AF31" s="136" t="s">
         <v>118</v>
       </c>
@@ -13529,7 +13532,7 @@
       </c>
     </row>
     <row r="32" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="640"/>
+      <c r="A32" s="650"/>
       <c r="B32" s="137" t="s">
         <v>119</v>
       </c>
@@ -13560,7 +13563,7 @@
         <f>Indata!I$16*10</f>
         <v>0</v>
       </c>
-      <c r="K32" s="640"/>
+      <c r="K32" s="650"/>
       <c r="L32" s="137" t="s">
         <v>119</v>
       </c>
@@ -13591,7 +13594,7 @@
         <f t="shared" si="65"/>
         <v>0</v>
       </c>
-      <c r="U32" s="640"/>
+      <c r="U32" s="650"/>
       <c r="V32" s="137" t="s">
         <v>119</v>
       </c>
@@ -13622,7 +13625,7 @@
         <f t="shared" si="70"/>
         <v>0</v>
       </c>
-      <c r="AE32" s="640"/>
+      <c r="AE32" s="650"/>
       <c r="AF32" s="137" t="s">
         <v>119</v>
       </c>
@@ -18503,6 +18506,40 @@
     </row>
   </sheetData>
   <mergeCells count="50">
+    <mergeCell ref="AE6:AE8"/>
+    <mergeCell ref="AE11:AE20"/>
+    <mergeCell ref="U29:U32"/>
+    <mergeCell ref="AE29:AE32"/>
+    <mergeCell ref="U23:U26"/>
+    <mergeCell ref="AE23:AE26"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="AE88:AE91"/>
+    <mergeCell ref="AE74:AE76"/>
+    <mergeCell ref="AE77:AE79"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="K11:K20"/>
+    <mergeCell ref="AE71:AE73"/>
+    <mergeCell ref="AE83:AE85"/>
+    <mergeCell ref="A36:A50"/>
+    <mergeCell ref="K36:K50"/>
+    <mergeCell ref="U36:U50"/>
+    <mergeCell ref="AE36:AE50"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="K29:K32"/>
+    <mergeCell ref="U11:U20"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="AF3:AG4"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
     <mergeCell ref="AE92:AE96"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C4"/>
@@ -18519,40 +18556,6 @@
     <mergeCell ref="K6:K8"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="K23:K26"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="AF3:AG4"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="AE88:AE91"/>
-    <mergeCell ref="AE74:AE76"/>
-    <mergeCell ref="AE77:AE79"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="K11:K20"/>
-    <mergeCell ref="AE71:AE73"/>
-    <mergeCell ref="AE83:AE85"/>
-    <mergeCell ref="A36:A50"/>
-    <mergeCell ref="K36:K50"/>
-    <mergeCell ref="U36:U50"/>
-    <mergeCell ref="AE36:AE50"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="K29:K32"/>
-    <mergeCell ref="U11:U20"/>
-    <mergeCell ref="AE6:AE8"/>
-    <mergeCell ref="AE11:AE20"/>
-    <mergeCell ref="U29:U32"/>
-    <mergeCell ref="AE29:AE32"/>
-    <mergeCell ref="U23:U26"/>
-    <mergeCell ref="AE23:AE26"/>
-    <mergeCell ref="U6:U8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -18566,8 +18569,8 @@
   </sheetPr>
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight" activeCell="D76" sqref="D76"/>
@@ -18620,18 +18623,18 @@
       <c r="A5" s="131"/>
       <c r="B5" s="132"/>
       <c r="C5" s="132"/>
-      <c r="D5" s="602" t="s">
+      <c r="D5" s="590" t="s">
         <v>64</v>
       </c>
-      <c r="E5" s="603"/>
-      <c r="F5" s="602" t="s">
+      <c r="E5" s="591"/>
+      <c r="F5" s="590" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="603"/>
-      <c r="H5" s="602" t="s">
+      <c r="G5" s="591"/>
+      <c r="H5" s="590" t="s">
         <v>66</v>
       </c>
-      <c r="I5" s="603"/>
+      <c r="I5" s="591"/>
       <c r="J5" s="598" t="s">
         <v>15</v>
       </c>
@@ -18651,18 +18654,18 @@
       </c>
       <c r="B6" s="138"/>
       <c r="C6" s="139"/>
-      <c r="D6" s="604" t="s">
+      <c r="D6" s="594" t="s">
         <v>337</v>
       </c>
-      <c r="E6" s="605"/>
-      <c r="F6" s="606" t="s">
+      <c r="E6" s="595"/>
+      <c r="F6" s="596" t="s">
         <v>382</v>
       </c>
-      <c r="G6" s="607"/>
-      <c r="H6" s="606" t="s">
+      <c r="G6" s="597"/>
+      <c r="H6" s="596" t="s">
         <v>382</v>
       </c>
-      <c r="I6" s="607"/>
+      <c r="I6" s="597"/>
       <c r="J6" s="65"/>
       <c r="K6" s="66"/>
       <c r="L6" s="66"/>
@@ -18757,7 +18760,7 @@
       <c r="S8" s="127"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="595" t="s">
+      <c r="A9" s="592" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="106" t="s">
@@ -18789,7 +18792,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="596"/>
+      <c r="A10" s="593"/>
       <c r="B10" s="43" t="s">
         <v>12</v>
       </c>
@@ -18819,7 +18822,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="596"/>
+      <c r="A11" s="593"/>
       <c r="B11" s="43" t="s">
         <v>13</v>
       </c>
@@ -18849,7 +18852,7 @@
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="596"/>
+      <c r="A12" s="593"/>
       <c r="B12" s="43" t="s">
         <v>37</v>
       </c>
@@ -18879,7 +18882,7 @@
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="595" t="s">
+      <c r="A13" s="592" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="106" t="s">
@@ -18911,7 +18914,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="597"/>
+      <c r="A14" s="600"/>
       <c r="B14" s="107" t="s">
         <v>9</v>
       </c>
@@ -18941,7 +18944,7 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="595" t="s">
+      <c r="A15" s="592" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="106" t="s">
@@ -18973,7 +18976,7 @@
       </c>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="597"/>
+      <c r="A16" s="600"/>
       <c r="B16" s="107" t="s">
         <v>324</v>
       </c>
@@ -19076,7 +19079,7 @@
       <c r="S18" s="127"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="595" t="s">
+      <c r="A19" s="592" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="106" t="s">
@@ -19108,7 +19111,7 @@
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="597"/>
+      <c r="A20" s="600"/>
       <c r="B20" s="107" t="s">
         <v>324</v>
       </c>
@@ -19138,7 +19141,7 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="596" t="s">
+      <c r="A21" s="593" t="s">
         <v>23</v>
       </c>
       <c r="B21" s="106" t="s">
@@ -19170,7 +19173,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="597"/>
+      <c r="A22" s="600"/>
       <c r="B22" s="107" t="s">
         <v>324</v>
       </c>
@@ -19273,7 +19276,7 @@
       <c r="S24" s="127"/>
     </row>
     <row r="25" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="595" t="s">
+      <c r="A25" s="592" t="s">
         <v>150</v>
       </c>
       <c r="B25" s="106" t="s">
@@ -19320,7 +19323,7 @@
       <c r="S25" s="26"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="596"/>
+      <c r="A26" s="593"/>
       <c r="B26" s="43" t="s">
         <v>9</v>
       </c>
@@ -19365,7 +19368,7 @@
       <c r="S26" s="26"/>
     </row>
     <row r="27" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="597"/>
+      <c r="A27" s="600"/>
       <c r="B27" s="107" t="s">
         <v>7</v>
       </c>
@@ -19457,7 +19460,7 @@
       <c r="S28" s="26"/>
     </row>
     <row r="29" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="595" t="s">
+      <c r="A29" s="592" t="s">
         <v>38</v>
       </c>
       <c r="B29" s="106" t="s">
@@ -19504,7 +19507,7 @@
       <c r="S29" s="26"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30" s="596"/>
+      <c r="A30" s="593"/>
       <c r="B30" s="43" t="s">
         <v>9</v>
       </c>
@@ -19549,7 +19552,7 @@
       <c r="S30" s="26"/>
     </row>
     <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="597"/>
+      <c r="A31" s="600"/>
       <c r="B31" s="107" t="s">
         <v>7</v>
       </c>
@@ -19594,7 +19597,7 @@
       <c r="S31" s="26"/>
     </row>
     <row r="32" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="590" t="s">
+      <c r="A32" s="601" t="s">
         <v>0</v>
       </c>
       <c r="B32" s="106" t="s">
@@ -19632,7 +19635,7 @@
       </c>
     </row>
     <row r="33" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="600"/>
+      <c r="A33" s="606"/>
       <c r="B33" s="43" t="s">
         <v>9</v>
       </c>
@@ -19668,7 +19671,7 @@
       </c>
     </row>
     <row r="34" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="600"/>
+      <c r="A34" s="606"/>
       <c r="B34" s="43" t="s">
         <v>7</v>
       </c>
@@ -19704,7 +19707,7 @@
       </c>
     </row>
     <row r="35" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="591"/>
+      <c r="A35" s="602"/>
       <c r="B35" s="107" t="s">
         <v>20</v>
       </c>
@@ -19867,7 +19870,7 @@
       <c r="S38" s="26"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="592" t="s">
+      <c r="A39" s="603" t="s">
         <v>27</v>
       </c>
       <c r="B39" s="106" t="s">
@@ -19913,7 +19916,7 @@
       <c r="S39" s="26"/>
     </row>
     <row r="40" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="601"/>
+      <c r="A40" s="607"/>
       <c r="B40" s="107" t="s">
         <v>29</v>
       </c>
@@ -19999,7 +20002,7 @@
       <c r="S41" s="127"/>
     </row>
     <row r="42" spans="1:19" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="590" t="s">
+      <c r="A42" s="601" t="s">
         <v>150</v>
       </c>
       <c r="B42" s="106" t="s">
@@ -20046,7 +20049,7 @@
       <c r="S42" s="26"/>
     </row>
     <row r="43" spans="1:19" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="600"/>
+      <c r="A43" s="606"/>
       <c r="B43" s="43" t="s">
         <v>117</v>
       </c>
@@ -20091,7 +20094,7 @@
       <c r="S43" s="26"/>
     </row>
     <row r="44" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="593"/>
+      <c r="A44" s="604"/>
       <c r="B44" s="43" t="s">
         <v>118</v>
       </c>
@@ -20136,7 +20139,7 @@
       <c r="S44" s="26"/>
     </row>
     <row r="45" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="593"/>
+      <c r="A45" s="604"/>
       <c r="B45" s="43" t="s">
         <v>119</v>
       </c>
@@ -20181,7 +20184,7 @@
       <c r="S45" s="26"/>
     </row>
     <row r="46" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="590" t="s">
+      <c r="A46" s="601" t="s">
         <v>381</v>
       </c>
       <c r="B46" s="106" t="s">
@@ -20228,7 +20231,7 @@
       <c r="S46" s="26"/>
     </row>
     <row r="47" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="600"/>
+      <c r="A47" s="606"/>
       <c r="B47" s="43" t="s">
         <v>117</v>
       </c>
@@ -20273,7 +20276,7 @@
       <c r="S47" s="26"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48" s="593"/>
+      <c r="A48" s="604"/>
       <c r="B48" s="43" t="s">
         <v>118</v>
       </c>
@@ -20318,7 +20321,7 @@
       <c r="S48" s="26"/>
     </row>
     <row r="49" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="593"/>
+      <c r="A49" s="604"/>
       <c r="B49" s="43" t="s">
         <v>119</v>
       </c>
@@ -20363,7 +20366,7 @@
       <c r="S49" s="26"/>
     </row>
     <row r="50" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="590" t="s">
+      <c r="A50" s="601" t="s">
         <v>380</v>
       </c>
       <c r="B50" s="106" t="s">
@@ -20410,7 +20413,7 @@
       <c r="S50" s="26"/>
     </row>
     <row r="51" spans="1:19" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="600"/>
+      <c r="A51" s="606"/>
       <c r="B51" s="43" t="s">
         <v>117</v>
       </c>
@@ -20455,7 +20458,7 @@
       <c r="S51" s="26"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52" s="593"/>
+      <c r="A52" s="604"/>
       <c r="B52" s="43" t="s">
         <v>118</v>
       </c>
@@ -20500,7 +20503,7 @@
       <c r="S52" s="26"/>
     </row>
     <row r="53" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="594"/>
+      <c r="A53" s="605"/>
       <c r="B53" s="107" t="s">
         <v>119</v>
       </c>
@@ -20545,7 +20548,7 @@
       <c r="S53" s="26"/>
     </row>
     <row r="54" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="600" t="s">
+      <c r="A54" s="606" t="s">
         <v>0</v>
       </c>
       <c r="B54" s="43" t="s">
@@ -20583,7 +20586,7 @@
       </c>
     </row>
     <row r="55" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="600"/>
+      <c r="A55" s="606"/>
       <c r="B55" s="43" t="s">
         <v>7</v>
       </c>
@@ -20619,7 +20622,7 @@
       </c>
     </row>
     <row r="56" spans="1:19" s="40" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="592" t="s">
+      <c r="A56" s="603" t="s">
         <v>17</v>
       </c>
       <c r="B56" s="342" t="s">
@@ -20657,7 +20660,7 @@
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A57" s="593"/>
+      <c r="A57" s="604"/>
       <c r="B57" s="43" t="s">
         <v>116</v>
       </c>
@@ -20702,7 +20705,7 @@
       <c r="S57" s="26"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A58" s="593"/>
+      <c r="A58" s="604"/>
       <c r="B58" s="43" t="s">
         <v>117</v>
       </c>
@@ -20747,7 +20750,7 @@
       <c r="S58" s="26"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A59" s="593"/>
+      <c r="A59" s="604"/>
       <c r="B59" s="43" t="s">
         <v>118</v>
       </c>
@@ -20792,7 +20795,7 @@
       <c r="S59" s="26"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="594"/>
+      <c r="A60" s="605"/>
       <c r="B60" s="107" t="s">
         <v>119</v>
       </c>
@@ -20912,7 +20915,7 @@
       <c r="K62" s="599"/>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A63" s="590" t="s">
+      <c r="A63" s="601" t="s">
         <v>312</v>
       </c>
       <c r="B63" s="106" t="s">
@@ -20950,7 +20953,7 @@
       </c>
     </row>
     <row r="64" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="591"/>
+      <c r="A64" s="602"/>
       <c r="B64" s="107" t="s">
         <v>7</v>
       </c>
@@ -21140,24 +21143,6 @@
     <protectedRange algorithmName="SHA-512" hashValue="bhbLMjBtLJkCl6+oRAIq98NZkcBAWzm8GjbRfoftLGnxxPl6tbwDiFe+9aTX2EHNMDT88cd1rnVmqQcow+/x8w==" saltValue="u4cWX+yqQiFBZXUHKrq6Og==" spinCount="100000" sqref="F9:I23" name="Indata"/>
   </protectedRanges>
   <mergeCells count="28">
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A25:A27"/>
     <mergeCell ref="A63:A64"/>
     <mergeCell ref="A56:A60"/>
     <mergeCell ref="A29:A31"/>
@@ -21168,6 +21153,24 @@
     <mergeCell ref="A39:A40"/>
     <mergeCell ref="A54:A55"/>
     <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -21200,11 +21203,11 @@
   </sheetPr>
   <dimension ref="A1:Q81"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D13" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="3" ySplit="6" topLeftCell="D59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F37" sqref="F37"/>
+      <selection pane="bottomRight" activeCell="G84" sqref="G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21290,18 +21293,18 @@
       <c r="C4" s="132" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="602" t="s">
+      <c r="D4" s="590" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="603"/>
-      <c r="F4" s="602" t="s">
+      <c r="E4" s="591"/>
+      <c r="F4" s="590" t="s">
         <v>65</v>
       </c>
-      <c r="G4" s="603"/>
-      <c r="H4" s="602" t="s">
+      <c r="G4" s="591"/>
+      <c r="H4" s="590" t="s">
         <v>66</v>
       </c>
-      <c r="I4" s="603"/>
+      <c r="I4" s="591"/>
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
       <c r="L4" s="40"/>
@@ -21317,21 +21320,21 @@
       </c>
       <c r="B5" s="290"/>
       <c r="C5" s="291"/>
-      <c r="D5" s="608" t="str">
+      <c r="D5" s="616" t="str">
         <f>Indata!D6</f>
         <v>Beslutad politik</v>
       </c>
-      <c r="E5" s="609"/>
-      <c r="F5" s="608" t="str">
+      <c r="E5" s="617"/>
+      <c r="F5" s="616" t="str">
         <f>Indata!F6</f>
         <v>Här kan användaren beskriva sitt scenario, t.ex. "Biodrivmedelsscenario"</v>
       </c>
-      <c r="G5" s="609"/>
-      <c r="H5" s="608" t="str">
+      <c r="G5" s="617"/>
+      <c r="H5" s="616" t="str">
         <f>Indata!H6</f>
         <v>Här kan användaren beskriva sitt scenario, t.ex. "Biodrivmedelsscenario"</v>
       </c>
-      <c r="I5" s="609"/>
+      <c r="I5" s="617"/>
       <c r="J5" s="66"/>
       <c r="K5" s="66"/>
       <c r="L5" s="66"/>
@@ -21379,7 +21382,7 @@
       <c r="Q6" s="127"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="610" t="s">
+      <c r="A7" s="611" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="292" t="s">
@@ -21513,7 +21516,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="611"/>
+      <c r="A11" s="613"/>
       <c r="B11" s="294" t="s">
         <v>185</v>
       </c>
@@ -21546,7 +21549,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="610" t="s">
+      <c r="A12" s="611" t="s">
         <v>38</v>
       </c>
       <c r="B12" s="292" t="s">
@@ -21681,7 +21684,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="611"/>
+      <c r="A16" s="613"/>
       <c r="B16" s="294" t="s">
         <v>323</v>
       </c>
@@ -21714,7 +21717,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="610" t="s">
+      <c r="A17" s="611" t="s">
         <v>21</v>
       </c>
       <c r="B17" s="292" t="s">
@@ -21749,7 +21752,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="611"/>
+      <c r="A18" s="613"/>
       <c r="B18" s="294" t="s">
         <v>324</v>
       </c>
@@ -21817,7 +21820,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="610" t="s">
+      <c r="A20" s="611" t="s">
         <v>77</v>
       </c>
       <c r="B20" s="292" t="s">
@@ -22022,7 +22025,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="611"/>
+      <c r="A26" s="613"/>
       <c r="B26" s="392" t="s">
         <v>359</v>
       </c>
@@ -22055,7 +22058,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="610" t="s">
+      <c r="A27" s="611" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="292" t="s">
@@ -22294,7 +22297,7 @@
       <c r="J33" s="381"/>
     </row>
     <row r="34" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="611"/>
+      <c r="A34" s="613"/>
       <c r="B34" s="392" t="s">
         <v>338</v>
       </c>
@@ -22363,7 +22366,7 @@
       </c>
     </row>
     <row r="36" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="611"/>
+      <c r="A36" s="613"/>
       <c r="B36" s="294" t="s">
         <v>324</v>
       </c>
@@ -22396,7 +22399,7 @@
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="616" t="s">
+      <c r="A37" s="614" t="s">
         <v>279</v>
       </c>
       <c r="B37" s="292" t="s">
@@ -22431,7 +22434,7 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="617"/>
+      <c r="A38" s="615"/>
       <c r="B38" s="293" t="s">
         <v>324</v>
       </c>
@@ -22464,7 +22467,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="617"/>
+      <c r="A39" s="615"/>
       <c r="B39" s="293" t="s">
         <v>315</v>
       </c>
@@ -22491,7 +22494,7 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="617"/>
+      <c r="A40" s="615"/>
       <c r="B40" s="391" t="s">
         <v>16</v>
       </c>
@@ -22524,7 +22527,7 @@
       </c>
     </row>
     <row r="41" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="617"/>
+      <c r="A41" s="615"/>
       <c r="B41" s="518" t="s">
         <v>362</v>
       </c>
@@ -22557,7 +22560,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="610" t="s">
+      <c r="A42" s="611" t="s">
         <v>276</v>
       </c>
       <c r="B42" s="292" t="s">
@@ -22828,7 +22831,7 @@
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" s="610" t="s">
+      <c r="A50" s="611" t="s">
         <v>271</v>
       </c>
       <c r="B50" s="292" t="s">
@@ -22962,7 +22965,7 @@
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" s="613" t="s">
+      <c r="A54" s="608" t="s">
         <v>130</v>
       </c>
       <c r="B54" s="292" t="s">
@@ -22998,7 +23001,7 @@
       <c r="J54" s="381"/>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A55" s="614"/>
+      <c r="A55" s="609"/>
       <c r="B55" s="293" t="s">
         <v>320</v>
       </c>
@@ -23033,7 +23036,7 @@
       <c r="K55" s="381"/>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" s="614"/>
+      <c r="A56" s="609"/>
       <c r="B56" s="293" t="s">
         <v>104</v>
       </c>
@@ -23068,7 +23071,7 @@
       <c r="K56" s="381"/>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="614"/>
+      <c r="A57" s="609"/>
       <c r="B57" s="293" t="s">
         <v>317</v>
       </c>
@@ -23107,7 +23110,7 @@
       <c r="O57" s="521"/>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" s="614"/>
+      <c r="A58" s="609"/>
       <c r="B58" s="293" t="s">
         <v>318</v>
       </c>
@@ -23142,7 +23145,7 @@
       <c r="K58" s="381"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" s="614"/>
+      <c r="A59" s="609"/>
       <c r="B59" s="293" t="s">
         <v>319</v>
       </c>
@@ -23178,7 +23181,7 @@
       <c r="O59" s="381"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" s="614"/>
+      <c r="A60" s="609"/>
       <c r="B60" s="391" t="s">
         <v>198</v>
       </c>
@@ -23217,7 +23220,7 @@
       <c r="O60" s="521"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" s="614"/>
+      <c r="A61" s="609"/>
       <c r="B61" s="391" t="s">
         <v>199</v>
       </c>
@@ -23252,7 +23255,7 @@
       <c r="K61" s="381"/>
     </row>
     <row r="62" spans="1:15" s="381" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="614"/>
+      <c r="A62" s="609"/>
       <c r="B62" s="391" t="s">
         <v>200</v>
       </c>
@@ -23285,7 +23288,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="615"/>
+      <c r="A63" s="610"/>
       <c r="B63" s="392" t="s">
         <v>364</v>
       </c>
@@ -23320,7 +23323,7 @@
       <c r="K63" s="381"/>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="614" t="s">
+      <c r="A64" s="609" t="s">
         <v>245</v>
       </c>
       <c r="B64" s="293" t="s">
@@ -23355,7 +23358,7 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="614"/>
+      <c r="A65" s="609"/>
       <c r="B65" s="293" t="s">
         <v>197</v>
       </c>
@@ -23388,7 +23391,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="614"/>
+      <c r="A66" s="609"/>
       <c r="B66" s="293" t="s">
         <v>104</v>
       </c>
@@ -23421,7 +23424,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="614"/>
+      <c r="A67" s="609"/>
       <c r="B67" s="293" t="s">
         <v>322</v>
       </c>
@@ -23454,7 +23457,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="614"/>
+      <c r="A68" s="609"/>
       <c r="B68" s="293" t="s">
         <v>321</v>
       </c>
@@ -23487,7 +23490,7 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="614"/>
+      <c r="A69" s="609"/>
       <c r="B69" s="293" t="s">
         <v>323</v>
       </c>
@@ -23520,7 +23523,7 @@
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="614"/>
+      <c r="A70" s="609"/>
       <c r="B70" s="391" t="s">
         <v>198</v>
       </c>
@@ -23553,7 +23556,7 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="614"/>
+      <c r="A71" s="609"/>
       <c r="B71" s="391" t="s">
         <v>199</v>
       </c>
@@ -23586,7 +23589,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="615"/>
+      <c r="A72" s="610"/>
       <c r="B72" s="392" t="s">
         <v>200</v>
       </c>
@@ -23619,7 +23622,7 @@
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="613" t="s">
+      <c r="A73" s="608" t="s">
         <v>203</v>
       </c>
       <c r="B73" s="292" t="s">
@@ -23654,7 +23657,7 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="614"/>
+      <c r="A74" s="609"/>
       <c r="B74" s="293" t="s">
         <v>324</v>
       </c>
@@ -23687,7 +23690,7 @@
       </c>
     </row>
     <row r="75" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="615"/>
+      <c r="A75" s="610"/>
       <c r="B75" s="392" t="s">
         <v>278</v>
       </c>
@@ -23720,7 +23723,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="613" t="s">
+      <c r="A76" s="608" t="s">
         <v>204</v>
       </c>
       <c r="B76" s="292" t="s">
@@ -23755,7 +23758,7 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="614"/>
+      <c r="A77" s="609"/>
       <c r="B77" s="293" t="s">
         <v>324</v>
       </c>
@@ -23788,7 +23791,7 @@
       </c>
     </row>
     <row r="78" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="615"/>
+      <c r="A78" s="610"/>
       <c r="B78" s="392" t="s">
         <v>278</v>
       </c>
@@ -23820,15 +23823,57 @@
         <v>24.86746127949721</v>
       </c>
     </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="26" t="s">
+        <v>410</v>
+      </c>
+      <c r="B79" s="292" t="s">
+        <v>187</v>
+      </c>
+      <c r="C79" s="292" t="s">
+        <v>136</v>
+      </c>
+      <c r="F79" s="26">
+        <f>D30*(D23-F23)+(F30-D30)*(F23-D23)/2</f>
+        <v>-3796.7756996424387</v>
+      </c>
+      <c r="G79" s="381">
+        <f>E30*(E23-G23)+(G30-E30)*(G23-E23)/2</f>
+        <v>100.42757139416648</v>
+      </c>
+    </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B80" s="293" t="s">
+        <v>324</v>
+      </c>
+      <c r="C80" s="296" t="s">
+        <v>136</v>
+      </c>
       <c r="E80" s="395"/>
       <c r="F80" s="395"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="392" t="s">
+        <v>278</v>
+      </c>
+      <c r="C81" s="392" t="s">
+        <v>136</v>
+      </c>
       <c r="D81" s="395"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="A12:A16"/>
     <mergeCell ref="A73:A75"/>
     <mergeCell ref="A76:A78"/>
     <mergeCell ref="A27:A34"/>
@@ -23838,17 +23883,6 @@
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A50:A52"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26015,13 +26049,13 @@
       <c r="O3" s="127"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="592" t="s">
+      <c r="A4" s="603" t="s">
         <v>294</v>
       </c>
-      <c r="B4" s="625" t="s">
+      <c r="B4" s="624" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="626"/>
+      <c r="C4" s="625"/>
       <c r="D4" s="326">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -26042,11 +26076,11 @@
       <c r="O4" s="40"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="622"/>
-      <c r="B5" s="627" t="s">
+      <c r="A5" s="628"/>
+      <c r="B5" s="626" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="628"/>
+      <c r="C5" s="627"/>
       <c r="D5" s="326">
         <v>-0.05</v>
       </c>
@@ -26067,11 +26101,11 @@
       <c r="O5" s="40"/>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="622"/>
-      <c r="B6" s="627" t="s">
+      <c r="A6" s="628"/>
+      <c r="B6" s="626" t="s">
         <v>176</v>
       </c>
-      <c r="C6" s="628"/>
+      <c r="C6" s="627"/>
       <c r="D6" s="326">
         <v>0</v>
       </c>
@@ -26092,11 +26126,11 @@
       <c r="O6" s="40"/>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="622"/>
-      <c r="B7" s="627" t="s">
+      <c r="A7" s="628"/>
+      <c r="B7" s="626" t="s">
         <v>177</v>
       </c>
-      <c r="C7" s="628"/>
+      <c r="C7" s="627"/>
       <c r="D7" s="326">
         <v>-0.1</v>
       </c>
@@ -26117,11 +26151,11 @@
       <c r="O7" s="40"/>
     </row>
     <row r="8" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="622"/>
-      <c r="B8" s="627" t="s">
+      <c r="A8" s="628"/>
+      <c r="B8" s="626" t="s">
         <v>178</v>
       </c>
-      <c r="C8" s="628"/>
+      <c r="C8" s="627"/>
       <c r="D8" s="326">
         <f>Indata!D80</f>
         <v>-0.2</v>
@@ -26143,11 +26177,11 @@
       <c r="O8" s="40"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="601"/>
-      <c r="B9" s="623" t="s">
+      <c r="A9" s="607"/>
+      <c r="B9" s="622" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="624"/>
+      <c r="C9" s="623"/>
       <c r="D9" s="328">
         <f>Indata!D78</f>
         <v>-0.22</v>
@@ -26169,7 +26203,7 @@
       <c r="O9" s="40"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="595" t="s">
+      <c r="A10" s="592" t="s">
         <v>265</v>
       </c>
       <c r="B10" s="106" t="s">
@@ -26198,7 +26232,7 @@
       <c r="O10" s="40"/>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="596"/>
+      <c r="A11" s="593"/>
       <c r="B11" s="43" t="s">
         <v>9</v>
       </c>
@@ -26225,7 +26259,7 @@
       <c r="O11" s="40"/>
     </row>
     <row r="12" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="596" t="s">
+      <c r="A12" s="593" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="43" t="s">
@@ -26254,7 +26288,7 @@
       <c r="O12" s="40"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="595" t="s">
+      <c r="A13" s="592" t="s">
         <v>266</v>
       </c>
       <c r="B13" s="106" t="s">
@@ -26283,7 +26317,7 @@
       <c r="O13" s="40"/>
     </row>
     <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="596"/>
+      <c r="A14" s="593"/>
       <c r="B14" s="43" t="s">
         <v>286</v>
       </c>
@@ -26310,7 +26344,7 @@
       <c r="O14" s="40"/>
     </row>
     <row r="15" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="596" t="s">
+      <c r="A15" s="593" t="s">
         <v>68</v>
       </c>
       <c r="B15" s="43" t="s">
@@ -26339,7 +26373,7 @@
       <c r="O15" s="40"/>
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="595" t="s">
+      <c r="A16" s="592" t="s">
         <v>272</v>
       </c>
       <c r="B16" s="106" t="s">
@@ -26368,7 +26402,7 @@
       <c r="O16" s="40"/>
     </row>
     <row r="17" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="596"/>
+      <c r="A17" s="593"/>
       <c r="B17" s="43" t="s">
         <v>286</v>
       </c>
@@ -26395,7 +26429,7 @@
       <c r="O17" s="40"/>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="597" t="s">
+      <c r="A18" s="600" t="s">
         <v>68</v>
       </c>
       <c r="B18" s="107" t="s">
@@ -26424,7 +26458,7 @@
       <c r="O18" s="40"/>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="614" t="s">
+      <c r="A19" s="609" t="s">
         <v>273</v>
       </c>
       <c r="B19" s="293" t="s">
@@ -26453,7 +26487,7 @@
       <c r="O19" s="40"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="614"/>
+      <c r="A20" s="609"/>
       <c r="B20" s="293" t="s">
         <v>296</v>
       </c>
@@ -26480,7 +26514,7 @@
       <c r="O20" s="40"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="590" t="s">
+      <c r="A21" s="601" t="s">
         <v>95</v>
       </c>
       <c r="B21" s="106" t="s">
@@ -26509,7 +26543,7 @@
       <c r="O21" s="40"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="600"/>
+      <c r="A22" s="606"/>
       <c r="B22" s="43" t="s">
         <v>97</v>
       </c>
@@ -26536,7 +26570,7 @@
       <c r="O22" s="40"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="600"/>
+      <c r="A23" s="606"/>
       <c r="B23" s="43" t="s">
         <v>134</v>
       </c>
@@ -26563,7 +26597,7 @@
       <c r="O23" s="40"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="600"/>
+      <c r="A24" s="606"/>
       <c r="B24" s="43" t="s">
         <v>98</v>
       </c>
@@ -26590,7 +26624,7 @@
       <c r="O24" s="40"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25" s="600"/>
+      <c r="A25" s="606"/>
       <c r="B25" s="43" t="s">
         <v>135</v>
       </c>
@@ -26617,7 +26651,7 @@
       <c r="O25" s="40"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="591"/>
+      <c r="A26" s="602"/>
       <c r="B26" s="107" t="s">
         <v>100</v>
       </c>
@@ -26645,6 +26679,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="A4:A9"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B4:C4"/>
@@ -26652,11 +26691,6 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A4:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26700,25 +26734,25 @@
       <c r="N1" s="40"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="632" t="s">
+      <c r="A2" s="629" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="632"/>
-      <c r="C2" s="632"/>
-      <c r="D2" s="632"/>
-      <c r="E2" s="632"/>
-      <c r="F2" s="632"/>
-      <c r="G2" s="632"/>
-      <c r="H2" s="632"/>
-      <c r="I2" s="632"/>
-      <c r="J2" s="632"/>
+      <c r="B2" s="629"/>
+      <c r="C2" s="629"/>
+      <c r="D2" s="629"/>
+      <c r="E2" s="629"/>
+      <c r="F2" s="629"/>
+      <c r="G2" s="629"/>
+      <c r="H2" s="629"/>
+      <c r="I2" s="629"/>
+      <c r="J2" s="629"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="633" t="s">
+      <c r="A3" s="630" t="s">
         <v>355</v>
       </c>
-      <c r="B3" s="634"/>
-      <c r="C3" s="634"/>
+      <c r="B3" s="631"/>
+      <c r="C3" s="631"/>
       <c r="D3" s="197"/>
       <c r="E3" s="197"/>
       <c r="F3" s="197"/>
@@ -26795,18 +26829,18 @@
       <c r="B7" s="194"/>
       <c r="C7" s="194"/>
       <c r="D7" s="194"/>
-      <c r="E7" s="629" t="s">
+      <c r="E7" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="630"/>
-      <c r="G7" s="629" t="s">
+      <c r="F7" s="633"/>
+      <c r="G7" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="H7" s="630"/>
-      <c r="I7" s="631" t="s">
+      <c r="H7" s="633"/>
+      <c r="I7" s="632" t="s">
         <v>66</v>
       </c>
-      <c r="J7" s="630"/>
+      <c r="J7" s="633"/>
       <c r="L7" s="26" t="s">
         <v>402</v>
       </c>
@@ -27422,18 +27456,18 @@
       <c r="B26" s="194"/>
       <c r="C26" s="194"/>
       <c r="D26" s="194"/>
-      <c r="E26" s="629" t="s">
+      <c r="E26" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="630"/>
-      <c r="G26" s="629" t="s">
+      <c r="F26" s="633"/>
+      <c r="G26" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="630"/>
-      <c r="I26" s="631" t="s">
+      <c r="H26" s="633"/>
+      <c r="I26" s="632" t="s">
         <v>66</v>
       </c>
-      <c r="J26" s="630"/>
+      <c r="J26" s="633"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="196" t="s">
@@ -28032,18 +28066,18 @@
       <c r="B45" s="194"/>
       <c r="C45" s="194"/>
       <c r="D45" s="194"/>
-      <c r="E45" s="629" t="s">
+      <c r="E45" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="630"/>
-      <c r="G45" s="629" t="s">
+      <c r="F45" s="633"/>
+      <c r="G45" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="H45" s="630"/>
-      <c r="I45" s="631" t="s">
+      <c r="H45" s="633"/>
+      <c r="I45" s="632" t="s">
         <v>66</v>
       </c>
-      <c r="J45" s="630"/>
+      <c r="J45" s="633"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="196" t="s">
@@ -28634,18 +28668,18 @@
       <c r="B64" s="194"/>
       <c r="C64" s="194"/>
       <c r="D64" s="194"/>
-      <c r="E64" s="629" t="s">
+      <c r="E64" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="F64" s="630"/>
-      <c r="G64" s="629" t="s">
+      <c r="F64" s="633"/>
+      <c r="G64" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="H64" s="630"/>
-      <c r="I64" s="631" t="s">
+      <c r="H64" s="633"/>
+      <c r="I64" s="632" t="s">
         <v>66</v>
       </c>
-      <c r="J64" s="630"/>
+      <c r="J64" s="633"/>
     </row>
     <row r="65" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="196" t="s">
@@ -29035,18 +29069,18 @@
       <c r="B77" s="194"/>
       <c r="C77" s="194"/>
       <c r="D77" s="194"/>
-      <c r="E77" s="629" t="s">
+      <c r="E77" s="634" t="s">
         <v>64</v>
       </c>
-      <c r="F77" s="630"/>
-      <c r="G77" s="629" t="s">
+      <c r="F77" s="633"/>
+      <c r="G77" s="634" t="s">
         <v>65</v>
       </c>
-      <c r="H77" s="630"/>
-      <c r="I77" s="631" t="s">
+      <c r="H77" s="633"/>
+      <c r="I77" s="632" t="s">
         <v>66</v>
       </c>
-      <c r="J77" s="630"/>
+      <c r="J77" s="633"/>
     </row>
     <row r="78" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="196" t="s">
@@ -29431,11 +29465,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="I45:J45"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="I26:J26"/>
     <mergeCell ref="G77:H77"/>
     <mergeCell ref="I77:J77"/>
     <mergeCell ref="E7:F7"/>
@@ -29448,6 +29477,11 @@
     <mergeCell ref="G45:H45"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="I26:J26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29498,87 +29532,87 @@
     </row>
     <row r="2" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:39" s="325" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="643" t="s">
+      <c r="A3" s="638" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="649" t="s">
+      <c r="B3" s="640" t="s">
         <v>226</v>
       </c>
-      <c r="C3" s="650"/>
-      <c r="D3" s="643" t="s">
+      <c r="C3" s="641"/>
+      <c r="D3" s="638" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="642"/>
-      <c r="F3" s="643" t="s">
+      <c r="E3" s="651"/>
+      <c r="F3" s="638" t="s">
         <v>65</v>
       </c>
-      <c r="G3" s="642"/>
-      <c r="H3" s="641" t="s">
+      <c r="G3" s="651"/>
+      <c r="H3" s="652" t="s">
         <v>66</v>
       </c>
-      <c r="I3" s="642"/>
-      <c r="K3" s="643" t="s">
+      <c r="I3" s="651"/>
+      <c r="K3" s="638" t="s">
         <v>67</v>
       </c>
       <c r="L3" s="644" t="s">
         <v>237</v>
       </c>
       <c r="M3" s="645"/>
-      <c r="N3" s="643" t="s">
+      <c r="N3" s="638" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="642"/>
-      <c r="P3" s="643" t="s">
+      <c r="O3" s="651"/>
+      <c r="P3" s="638" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="642"/>
-      <c r="R3" s="641" t="s">
+      <c r="Q3" s="651"/>
+      <c r="R3" s="652" t="s">
         <v>66</v>
       </c>
-      <c r="S3" s="642"/>
-      <c r="U3" s="643" t="s">
+      <c r="S3" s="651"/>
+      <c r="U3" s="638" t="s">
         <v>67</v>
       </c>
       <c r="V3" s="644" t="s">
         <v>227</v>
       </c>
       <c r="W3" s="645"/>
-      <c r="X3" s="643" t="s">
+      <c r="X3" s="638" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="642"/>
-      <c r="Z3" s="643" t="s">
+      <c r="Y3" s="651"/>
+      <c r="Z3" s="638" t="s">
         <v>65</v>
       </c>
-      <c r="AA3" s="642"/>
-      <c r="AB3" s="641" t="s">
+      <c r="AA3" s="651"/>
+      <c r="AB3" s="652" t="s">
         <v>66</v>
       </c>
-      <c r="AC3" s="642"/>
-      <c r="AE3" s="643" t="s">
+      <c r="AC3" s="651"/>
+      <c r="AE3" s="638" t="s">
         <v>67</v>
       </c>
       <c r="AF3" s="644" t="s">
         <v>238</v>
       </c>
       <c r="AG3" s="645"/>
-      <c r="AH3" s="643" t="s">
+      <c r="AH3" s="638" t="s">
         <v>64</v>
       </c>
-      <c r="AI3" s="642"/>
-      <c r="AJ3" s="643" t="s">
+      <c r="AI3" s="651"/>
+      <c r="AJ3" s="638" t="s">
         <v>65</v>
       </c>
-      <c r="AK3" s="642"/>
-      <c r="AL3" s="641" t="s">
+      <c r="AK3" s="651"/>
+      <c r="AL3" s="652" t="s">
         <v>66</v>
       </c>
-      <c r="AM3" s="642"/>
+      <c r="AM3" s="651"/>
     </row>
     <row r="4" spans="1:39" s="127" customFormat="1" ht="25.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="648"/>
-      <c r="B4" s="651"/>
-      <c r="C4" s="652"/>
+      <c r="A4" s="639"/>
+      <c r="B4" s="642"/>
+      <c r="C4" s="643"/>
       <c r="D4" s="265">
         <v>2030</v>
       </c>
@@ -29597,7 +29631,7 @@
       <c r="I4" s="266">
         <v>2040</v>
       </c>
-      <c r="K4" s="648"/>
+      <c r="K4" s="639"/>
       <c r="L4" s="646"/>
       <c r="M4" s="647"/>
       <c r="N4" s="265">
@@ -29618,7 +29652,7 @@
       <c r="S4" s="266">
         <v>2040</v>
       </c>
-      <c r="U4" s="648"/>
+      <c r="U4" s="639"/>
       <c r="V4" s="646"/>
       <c r="W4" s="647"/>
       <c r="X4" s="265">
@@ -29639,7 +29673,7 @@
       <c r="AC4" s="266">
         <v>2040</v>
       </c>
-      <c r="AE4" s="648"/>
+      <c r="AE4" s="639"/>
       <c r="AF4" s="646"/>
       <c r="AG4" s="647"/>
       <c r="AH4" s="265">
@@ -29702,7 +29736,7 @@
       <c r="AM5" s="201"/>
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A6" s="638" t="s">
+      <c r="A6" s="648" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="135" t="s">
@@ -29735,7 +29769,7 @@
         <f>Indata!I32</f>
         <v>21.293751803814949</v>
       </c>
-      <c r="K6" s="638" t="s">
+      <c r="K6" s="648" t="s">
         <v>0</v>
       </c>
       <c r="L6" s="135" t="s">
@@ -29768,7 +29802,7 @@
         <f>'Modell - Drivmedelpriser'!J24</f>
         <v>27.329509698551796</v>
       </c>
-      <c r="U6" s="638" t="s">
+      <c r="U6" s="648" t="s">
         <v>0</v>
       </c>
       <c r="V6" s="135" t="s">
@@ -29801,7 +29835,7 @@
         <f t="shared" ref="AC6:AC8" si="4">S6</f>
         <v>27.329509698551796</v>
       </c>
-      <c r="AE6" s="638" t="s">
+      <c r="AE6" s="648" t="s">
         <v>0</v>
       </c>
       <c r="AF6" s="135" t="s">
@@ -29836,7 +29870,7 @@
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A7" s="639"/>
+      <c r="A7" s="649"/>
       <c r="B7" s="136" t="s">
         <v>9</v>
       </c>
@@ -29867,7 +29901,7 @@
         <f>Indata!I33</f>
         <v>22.557131724953557</v>
       </c>
-      <c r="K7" s="639"/>
+      <c r="K7" s="649"/>
       <c r="L7" s="136" t="s">
         <v>9</v>
       </c>
@@ -29898,7 +29932,7 @@
         <f>'Modell - Drivmedelpriser'!J43</f>
         <v>24.89327119863777</v>
       </c>
-      <c r="U7" s="639"/>
+      <c r="U7" s="649"/>
       <c r="V7" s="136" t="s">
         <v>9</v>
       </c>
@@ -29929,7 +29963,7 @@
         <f t="shared" si="4"/>
         <v>24.89327119863777</v>
       </c>
-      <c r="AE7" s="639"/>
+      <c r="AE7" s="649"/>
       <c r="AF7" s="136" t="s">
         <v>9</v>
       </c>
@@ -29962,7 +29996,7 @@
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="639"/>
+      <c r="A8" s="649"/>
       <c r="B8" s="136" t="s">
         <v>7</v>
       </c>
@@ -29993,7 +30027,7 @@
         <f>Indata!I34</f>
         <v>4.1598749999999995</v>
       </c>
-      <c r="K8" s="639"/>
+      <c r="K8" s="649"/>
       <c r="L8" s="136" t="s">
         <v>7</v>
       </c>
@@ -30024,7 +30058,7 @@
         <f>'Modell - Drivmedelpriser'!J75</f>
         <v>4.1598749999999995</v>
       </c>
-      <c r="U8" s="639"/>
+      <c r="U8" s="649"/>
       <c r="V8" s="136" t="s">
         <v>7</v>
       </c>
@@ -30055,7 +30089,7 @@
         <f t="shared" si="4"/>
         <v>4.1598749999999995</v>
       </c>
-      <c r="AE8" s="639"/>
+      <c r="AE8" s="649"/>
       <c r="AF8" s="136" t="s">
         <v>7</v>
       </c>
@@ -30088,7 +30122,7 @@
       </c>
     </row>
     <row r="9" spans="1:39" s="303" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="639"/>
+      <c r="A9" s="649"/>
       <c r="B9" s="187" t="s">
         <v>20</v>
       </c>
@@ -30119,7 +30153,7 @@
         <f>Indata!I35</f>
         <v>21.888963239913203</v>
       </c>
-      <c r="K9" s="639"/>
+      <c r="K9" s="649"/>
       <c r="L9" s="187" t="s">
         <v>20</v>
       </c>
@@ -30150,7 +30184,7 @@
         <f t="shared" si="12"/>
         <v>26.181733806320725</v>
       </c>
-      <c r="U9" s="639"/>
+      <c r="U9" s="649"/>
       <c r="V9" s="187" t="s">
         <v>20</v>
       </c>
@@ -30181,7 +30215,7 @@
         <f t="shared" si="13"/>
         <v>26.181733806320722</v>
       </c>
-      <c r="AE9" s="639"/>
+      <c r="AE9" s="649"/>
       <c r="AF9" s="187" t="s">
         <v>20</v>
       </c>
@@ -30214,7 +30248,7 @@
       </c>
     </row>
     <row r="10" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="640"/>
+      <c r="A10" s="650"/>
       <c r="B10" s="188" t="s">
         <v>234</v>
       </c>
@@ -30239,7 +30273,7 @@
       <c r="I10" s="225" t="s">
         <v>78</v>
       </c>
-      <c r="K10" s="640"/>
+      <c r="K10" s="650"/>
       <c r="L10" s="188" t="s">
         <v>234</v>
       </c>
@@ -30270,7 +30304,7 @@
         <f t="shared" si="15"/>
         <v>0.1961157556599078</v>
       </c>
-      <c r="U10" s="640"/>
+      <c r="U10" s="650"/>
       <c r="V10" s="188" t="s">
         <v>234</v>
       </c>
@@ -30301,7 +30335,7 @@
         <f t="shared" si="16"/>
         <v>0.1961157556599078</v>
       </c>
-      <c r="AE10" s="640"/>
+      <c r="AE10" s="650"/>
       <c r="AF10" s="188" t="s">
         <v>234</v>
       </c>
@@ -30403,7 +30437,7 @@
       <c r="AM12" s="201"/>
     </row>
     <row r="13" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="638" t="s">
+      <c r="A13" s="648" t="s">
         <v>38</v>
       </c>
       <c r="B13" s="135" t="s">
@@ -30436,7 +30470,7 @@
         <f>Indata!I29</f>
         <v>0.49219920755019081</v>
       </c>
-      <c r="K13" s="638" t="s">
+      <c r="K13" s="648" t="s">
         <v>38</v>
       </c>
       <c r="L13" s="135" t="s">
@@ -30469,7 +30503,7 @@
         <f>I13*(100%+S$10*'Indata - Effektsamband-Faktorer'!$E$5)*(1-Indata!I$19)</f>
         <v>0.48737280657399518</v>
       </c>
-      <c r="U13" s="638" t="s">
+      <c r="U13" s="648" t="s">
         <v>38</v>
       </c>
       <c r="V13" s="135" t="s">
@@ -30502,7 +30536,7 @@
         <f t="shared" ref="AC13:AC15" si="22">S13</f>
         <v>0.48737280657399518</v>
       </c>
-      <c r="AE13" s="638" t="s">
+      <c r="AE13" s="648" t="s">
         <v>38</v>
       </c>
       <c r="AF13" s="135" t="s">
@@ -30537,7 +30571,7 @@
       </c>
     </row>
     <row r="14" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A14" s="639"/>
+      <c r="A14" s="649"/>
       <c r="B14" s="136" t="s">
         <v>9</v>
       </c>
@@ -30568,7 +30602,7 @@
         <f>Indata!I30</f>
         <v>0.49160078067679608</v>
       </c>
-      <c r="K14" s="639"/>
+      <c r="K14" s="649"/>
       <c r="L14" s="136" t="s">
         <v>9</v>
       </c>
@@ -30599,7 +30633,7 @@
         <f>I14*(100%+S$10*'Indata - Effektsamband-Faktorer'!$E$5)*(1-Indata!I$19)</f>
         <v>0.4867802477475246</v>
       </c>
-      <c r="U14" s="639"/>
+      <c r="U14" s="649"/>
       <c r="V14" s="136" t="s">
         <v>9</v>
       </c>
@@ -30630,7 +30664,7 @@
         <f t="shared" si="22"/>
         <v>0.4867802477475246</v>
       </c>
-      <c r="AE14" s="639"/>
+      <c r="AE14" s="649"/>
       <c r="AF14" s="136" t="s">
         <v>9</v>
       </c>
@@ -30663,7 +30697,7 @@
       </c>
     </row>
     <row r="15" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="640"/>
+      <c r="A15" s="650"/>
       <c r="B15" s="137" t="s">
         <v>7</v>
       </c>
@@ -30694,7 +30728,7 @@
         <f>Indata!I31</f>
         <v>1.6150000000000002</v>
       </c>
-      <c r="K15" s="640"/>
+      <c r="K15" s="650"/>
       <c r="L15" s="137" t="s">
         <v>7</v>
       </c>
@@ -30725,7 +30759,7 @@
         <f>I15*(1-Indata!I$19)</f>
         <v>1.6150000000000002</v>
       </c>
-      <c r="U15" s="640"/>
+      <c r="U15" s="650"/>
       <c r="V15" s="137" t="s">
         <v>7</v>
       </c>
@@ -30756,7 +30790,7 @@
         <f t="shared" si="22"/>
         <v>1.6150000000000002</v>
       </c>
-      <c r="AE15" s="640"/>
+      <c r="AE15" s="650"/>
       <c r="AF15" s="137" t="s">
         <v>7</v>
       </c>
@@ -31439,7 +31473,7 @@
       <c r="AM23" s="201"/>
     </row>
     <row r="24" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="638" t="s">
+      <c r="A24" s="648" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="135" t="s">
@@ -31472,7 +31506,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K24" s="638" t="s">
+      <c r="K24" s="648" t="s">
         <v>21</v>
       </c>
       <c r="L24" s="135" t="s">
@@ -31505,7 +31539,7 @@
         <f t="shared" si="45"/>
         <v>0</v>
       </c>
-      <c r="U24" s="638" t="s">
+      <c r="U24" s="648" t="s">
         <v>21</v>
       </c>
       <c r="V24" s="135" t="s">
@@ -31538,7 +31572,7 @@
         <f t="shared" ref="AC24:AC26" si="50">S24</f>
         <v>0</v>
       </c>
-      <c r="AE24" s="638" t="s">
+      <c r="AE24" s="648" t="s">
         <v>21</v>
       </c>
       <c r="AF24" s="135" t="s">
@@ -31573,7 +31607,7 @@
       </c>
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A25" s="639"/>
+      <c r="A25" s="649"/>
       <c r="B25" s="136" t="s">
         <v>9</v>
       </c>
@@ -31604,7 +31638,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K25" s="639"/>
+      <c r="K25" s="649"/>
       <c r="L25" s="136" t="s">
         <v>9</v>
       </c>
@@ -31635,7 +31669,7 @@
         <f t="shared" ref="S25:S26" si="61">I25</f>
         <v>0</v>
       </c>
-      <c r="U25" s="639"/>
+      <c r="U25" s="649"/>
       <c r="V25" s="136" t="s">
         <v>9</v>
       </c>
@@ -31666,7 +31700,7 @@
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AE25" s="639"/>
+      <c r="AE25" s="649"/>
       <c r="AF25" s="136" t="s">
         <v>9</v>
       </c>
@@ -31699,7 +31733,7 @@
       </c>
     </row>
     <row r="26" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="640"/>
+      <c r="A26" s="650"/>
       <c r="B26" s="137" t="s">
         <v>7</v>
       </c>
@@ -31730,7 +31764,7 @@
         <f>Indata!I$15*10</f>
         <v>0</v>
       </c>
-      <c r="K26" s="640"/>
+      <c r="K26" s="650"/>
       <c r="L26" s="137" t="s">
         <v>7</v>
       </c>
@@ -31761,7 +31795,7 @@
         <f t="shared" si="61"/>
         <v>0</v>
       </c>
-      <c r="U26" s="640"/>
+      <c r="U26" s="650"/>
       <c r="V26" s="137" t="s">
         <v>7</v>
       </c>
@@ -31792,7 +31826,7 @@
         <f t="shared" si="50"/>
         <v>0</v>
       </c>
-      <c r="AE26" s="640"/>
+      <c r="AE26" s="650"/>
       <c r="AF26" s="137" t="s">
         <v>7</v>
       </c>
@@ -31900,7 +31934,7 @@
       <c r="AM28" s="201"/>
     </row>
     <row r="29" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="638" t="s">
+      <c r="A29" s="648" t="s">
         <v>75</v>
       </c>
       <c r="B29" s="135" t="s">
@@ -31933,7 +31967,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K29" s="638" t="s">
+      <c r="K29" s="648" t="s">
         <v>75</v>
       </c>
       <c r="L29" s="135" t="s">
@@ -31966,7 +32000,7 @@
         <f t="shared" ref="S29:S31" si="68">I29</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="U29" s="638" t="s">
+      <c r="U29" s="648" t="s">
         <v>75</v>
       </c>
       <c r="V29" s="135" t="s">
@@ -31999,7 +32033,7 @@
         <f t="shared" ref="AC29:AC31" si="73">S29</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE29" s="638" t="s">
+      <c r="AE29" s="648" t="s">
         <v>75</v>
       </c>
       <c r="AF29" s="135" t="s">
@@ -32034,7 +32068,7 @@
       </c>
     </row>
     <row r="30" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A30" s="639"/>
+      <c r="A30" s="649"/>
       <c r="B30" s="136" t="s">
         <v>9</v>
       </c>
@@ -32065,7 +32099,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K30" s="639"/>
+      <c r="K30" s="649"/>
       <c r="L30" s="136" t="s">
         <v>9</v>
       </c>
@@ -32096,7 +32130,7 @@
         <f t="shared" si="68"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="U30" s="639"/>
+      <c r="U30" s="649"/>
       <c r="V30" s="136" t="s">
         <v>9</v>
       </c>
@@ -32127,7 +32161,7 @@
         <f t="shared" si="73"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE30" s="639"/>
+      <c r="AE30" s="649"/>
       <c r="AF30" s="136" t="s">
         <v>9</v>
       </c>
@@ -32160,7 +32194,7 @@
       </c>
     </row>
     <row r="31" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="640"/>
+      <c r="A31" s="650"/>
       <c r="B31" s="137" t="s">
         <v>7</v>
       </c>
@@ -32191,7 +32225,7 @@
         <f>Indata!I$36</f>
         <v>10.009999999999998</v>
       </c>
-      <c r="K31" s="640"/>
+      <c r="K31" s="650"/>
       <c r="L31" s="137" t="s">
         <v>7</v>
       </c>
@@ -32222,7 +32256,7 @@
         <f t="shared" si="68"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="U31" s="640"/>
+      <c r="U31" s="650"/>
       <c r="V31" s="137" t="s">
         <v>7</v>
       </c>
@@ -32253,7 +32287,7 @@
         <f t="shared" si="73"/>
         <v>10.009999999999998</v>
       </c>
-      <c r="AE31" s="640"/>
+      <c r="AE31" s="650"/>
       <c r="AF31" s="137" t="s">
         <v>7</v>
       </c>
@@ -32944,7 +32978,7 @@
       <c r="AM39" s="201"/>
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A40" s="638" t="s">
+      <c r="A40" s="648" t="s">
         <v>77</v>
       </c>
       <c r="B40" s="135" t="s">
@@ -32977,7 +33011,7 @@
         <f t="shared" si="90"/>
         <v>20.490767763608162</v>
       </c>
-      <c r="K40" s="638" t="s">
+      <c r="K40" s="648" t="s">
         <v>77</v>
       </c>
       <c r="L40" s="135" t="s">
@@ -33010,7 +33044,7 @@
         <f t="shared" si="91"/>
         <v>23.329659844074406</v>
       </c>
-      <c r="U40" s="638" t="s">
+      <c r="U40" s="648" t="s">
         <v>77</v>
       </c>
       <c r="V40" s="135" t="s">
@@ -33043,7 +33077,7 @@
         <f t="shared" ref="AC40:AC42" si="96">S40</f>
         <v>23.329659844074406</v>
       </c>
-      <c r="AE40" s="638" t="s">
+      <c r="AE40" s="648" t="s">
         <v>77</v>
       </c>
       <c r="AF40" s="135" t="s">
@@ -33078,7 +33112,7 @@
       </c>
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A41" s="639"/>
+      <c r="A41" s="649"/>
       <c r="B41" s="136" t="s">
         <v>9</v>
       </c>
@@ -33109,7 +33143,7 @@
         <f t="shared" si="90"/>
         <v>21.099103565816492</v>
       </c>
-      <c r="K41" s="639"/>
+      <c r="K41" s="649"/>
       <c r="L41" s="136" t="s">
         <v>9</v>
       </c>
@@ -33140,7 +33174,7 @@
         <f t="shared" si="91"/>
         <v>22.127552721319212</v>
       </c>
-      <c r="U41" s="639"/>
+      <c r="U41" s="649"/>
       <c r="V41" s="136" t="s">
         <v>9</v>
       </c>
@@ -33171,7 +33205,7 @@
         <f t="shared" si="96"/>
         <v>22.127552721319212</v>
       </c>
-      <c r="AE41" s="639"/>
+      <c r="AE41" s="649"/>
       <c r="AF41" s="136" t="s">
         <v>9</v>
       </c>
@@ -33204,7 +33238,7 @@
       </c>
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A42" s="639"/>
+      <c r="A42" s="649"/>
       <c r="B42" s="136" t="s">
         <v>7</v>
       </c>
@@ -33235,7 +33269,7 @@
         <f t="shared" si="90"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="K42" s="639"/>
+      <c r="K42" s="649"/>
       <c r="L42" s="136" t="s">
         <v>7</v>
       </c>
@@ -33266,7 +33300,7 @@
         <f t="shared" si="91"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="U42" s="639"/>
+      <c r="U42" s="649"/>
       <c r="V42" s="136" t="s">
         <v>7</v>
       </c>
@@ -33297,7 +33331,7 @@
         <f t="shared" si="96"/>
         <v>16.728198124999999</v>
       </c>
-      <c r="AE42" s="639"/>
+      <c r="AE42" s="649"/>
       <c r="AF42" s="136" t="s">
         <v>7</v>
       </c>
@@ -33330,7 +33364,7 @@
       </c>
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A43" s="639"/>
+      <c r="A43" s="649"/>
       <c r="B43" s="187" t="s">
         <v>76</v>
       </c>
@@ -33359,7 +33393,7 @@
         <f t="shared" si="104"/>
         <v>18.064425082921922</v>
       </c>
-      <c r="K43" s="639"/>
+      <c r="K43" s="649"/>
       <c r="L43" s="187" t="s">
         <v>76</v>
       </c>
@@ -33390,7 +33424,7 @@
         <f t="shared" ref="S43" si="105">SUMPRODUCT(S40:S42,S34:S36)/S37</f>
         <v>18.645576333860959</v>
       </c>
-      <c r="U43" s="639"/>
+      <c r="U43" s="649"/>
       <c r="V43" s="187" t="s">
         <v>76</v>
       </c>
@@ -33421,7 +33455,7 @@
         <f t="shared" si="106"/>
         <v>18.645576333860962</v>
       </c>
-      <c r="AE43" s="639"/>
+      <c r="AE43" s="649"/>
       <c r="AF43" s="187" t="s">
         <v>76</v>
       </c>
@@ -33454,7 +33488,7 @@
       </c>
     </row>
     <row r="44" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="640"/>
+      <c r="A44" s="650"/>
       <c r="B44" s="188" t="s">
         <v>234</v>
       </c>
@@ -33479,7 +33513,7 @@
       <c r="I44" s="225" t="s">
         <v>78</v>
       </c>
-      <c r="K44" s="640"/>
+      <c r="K44" s="650"/>
       <c r="L44" s="188" t="s">
         <v>234</v>
       </c>
@@ -33510,7 +33544,7 @@
         <f>S43/E43-1</f>
         <v>-5.1358020489668088E-2</v>
       </c>
-      <c r="U44" s="640"/>
+      <c r="U44" s="650"/>
       <c r="V44" s="188" t="s">
         <v>234</v>
       </c>
@@ -33541,7 +33575,7 @@
         <f>AC43/E43-1</f>
         <v>-5.1358020489667866E-2</v>
       </c>
-      <c r="AE44" s="640"/>
+      <c r="AE44" s="650"/>
       <c r="AF44" s="188" t="s">
         <v>234</v>
       </c>
@@ -33649,7 +33683,7 @@
       <c r="AM46" s="78"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A47" s="638" t="s">
+      <c r="A47" s="648" t="s">
         <v>29</v>
       </c>
       <c r="B47" s="135" t="s">
@@ -33682,7 +33716,7 @@
         <f>Indata!I39</f>
         <v>11648700</v>
       </c>
-      <c r="K47" s="638" t="s">
+      <c r="K47" s="648" t="s">
         <v>29</v>
       </c>
       <c r="L47" s="135" t="s">
@@ -33715,7 +33749,7 @@
         <f t="shared" si="107"/>
         <v>11648700</v>
       </c>
-      <c r="U47" s="638" t="s">
+      <c r="U47" s="648" t="s">
         <v>29</v>
       </c>
       <c r="V47" s="135" t="s">
@@ -33748,7 +33782,7 @@
         <f t="shared" ref="AC47:AC49" si="112">S47</f>
         <v>11648700</v>
       </c>
-      <c r="AE47" s="638" t="s">
+      <c r="AE47" s="648" t="s">
         <v>29</v>
       </c>
       <c r="AF47" s="135" t="s">
@@ -33783,7 +33817,7 @@
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A48" s="639"/>
+      <c r="A48" s="649"/>
       <c r="B48" s="136" t="s">
         <v>29</v>
       </c>
@@ -33814,7 +33848,7 @@
         <f>Indata!I40</f>
         <v>0.52928701904391762</v>
       </c>
-      <c r="K48" s="639"/>
+      <c r="K48" s="649"/>
       <c r="L48" s="136" t="s">
         <v>29</v>
       </c>
@@ -33845,7 +33879,7 @@
         <f>(1+'Indata - Effektsamband-Faktorer'!$E$7*S44)*'Modell - Lätta fordon'!I48</f>
         <v>0.53200533240081493</v>
       </c>
-      <c r="U48" s="639"/>
+      <c r="U48" s="649"/>
       <c r="V48" s="136" t="s">
         <v>29</v>
       </c>
@@ -33876,7 +33910,7 @@
         <f t="shared" si="112"/>
         <v>0.53200533240081493</v>
       </c>
-      <c r="AE48" s="639"/>
+      <c r="AE48" s="649"/>
       <c r="AF48" s="136" t="s">
         <v>29</v>
       </c>
@@ -33909,7 +33943,7 @@
       </c>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A49" s="639"/>
+      <c r="A49" s="649"/>
       <c r="B49" s="136" t="s">
         <v>34</v>
       </c>
@@ -33940,7 +33974,7 @@
         <f t="shared" si="118"/>
         <v>6165505.6987368828</v>
       </c>
-      <c r="K49" s="639"/>
+      <c r="K49" s="649"/>
       <c r="L49" s="136" t="s">
         <v>34</v>
       </c>
@@ -33971,7 +34005,7 @@
         <f t="shared" ref="S49" si="121">S47*S48</f>
         <v>6197170.5155373728</v>
       </c>
-      <c r="U49" s="639"/>
+      <c r="U49" s="649"/>
       <c r="V49" s="136" t="s">
         <v>34</v>
       </c>
@@ -34002,7 +34036,7 @@
         <f t="shared" si="112"/>
         <v>6197170.5155373728</v>
       </c>
-      <c r="AE49" s="639"/>
+      <c r="AE49" s="649"/>
       <c r="AF49" s="136" t="s">
         <v>34</v>
       </c>
@@ -34035,7 +34069,7 @@
       </c>
     </row>
     <row r="50" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="640"/>
+      <c r="A50" s="650"/>
       <c r="B50" s="188" t="s">
         <v>234</v>
       </c>
@@ -34060,7 +34094,7 @@
       <c r="I50" s="225" t="s">
         <v>78</v>
       </c>
-      <c r="K50" s="640"/>
+      <c r="K50" s="650"/>
       <c r="L50" s="188" t="s">
         <v>234</v>
       </c>
@@ -34091,7 +34125,7 @@
         <f>S49/E49-1</f>
         <v>5.1358020489669087E-3</v>
       </c>
-      <c r="U50" s="640"/>
+      <c r="U50" s="650"/>
       <c r="V50" s="188" t="s">
         <v>234</v>
       </c>
@@ -34122,7 +34156,7 @@
         <f>AC49/E49-1</f>
         <v>5.1358020489669087E-3</v>
       </c>
-      <c r="AE50" s="640"/>
+      <c r="AE50" s="650"/>
       <c r="AF50" s="188" t="s">
         <v>234</v>
       </c>
@@ -35686,6 +35720,48 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="AE57:AE60"/>
+    <mergeCell ref="AE61:AE64"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="K18:K21"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="U18:U21"/>
+    <mergeCell ref="U24:U26"/>
+    <mergeCell ref="U29:U31"/>
+    <mergeCell ref="U34:U37"/>
+    <mergeCell ref="U40:U44"/>
+    <mergeCell ref="U47:U50"/>
+    <mergeCell ref="AE34:AE37"/>
+    <mergeCell ref="AE40:AE44"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="K47:K50"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="A47:A50"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="K34:K37"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="K24:K26"/>
+    <mergeCell ref="K29:K31"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AB3:AC3"/>
+    <mergeCell ref="U6:U10"/>
+    <mergeCell ref="U13:U15"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AE6:AE10"/>
+    <mergeCell ref="AE13:AE15"/>
+    <mergeCell ref="AF3:AG4"/>
     <mergeCell ref="AE86:AE89"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:C4"/>
@@ -35702,48 +35778,6 @@
     <mergeCell ref="AE24:AE26"/>
     <mergeCell ref="AE29:AE31"/>
     <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AE6:AE10"/>
-    <mergeCell ref="AE13:AE15"/>
-    <mergeCell ref="AF3:AG4"/>
-    <mergeCell ref="Z3:AA3"/>
-    <mergeCell ref="AB3:AC3"/>
-    <mergeCell ref="U6:U10"/>
-    <mergeCell ref="U13:U15"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="K47:K50"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="K40:K44"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="A47:A50"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="K34:K37"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="K24:K26"/>
-    <mergeCell ref="K29:K31"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="AE57:AE60"/>
-    <mergeCell ref="AE61:AE64"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="K18:K21"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="U18:U21"/>
-    <mergeCell ref="U24:U26"/>
-    <mergeCell ref="U29:U31"/>
-    <mergeCell ref="U34:U37"/>
-    <mergeCell ref="U40:U44"/>
-    <mergeCell ref="U47:U50"/>
-    <mergeCell ref="AE34:AE37"/>
-    <mergeCell ref="AE40:AE44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>